<commit_message>
more changes on export
</commit_message>
<xml_diff>
--- a/templates/excel_template/dreams_export.xlsx
+++ b/templates/excel_template/dreams_export.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13680" yWindow="460" windowWidth="14540" windowHeight="22320"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22280" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Enrollment" sheetId="1" r:id="rId1"/>
-    <sheet name="Interventions" sheetId="2" r:id="rId2"/>
+    <sheet name="enrollment_refined" sheetId="3" r:id="rId2"/>
+    <sheet name="Interventions" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="383">
   <si>
     <t>Table 1</t>
   </si>
@@ -628,6 +629,555 @@
   </si>
   <si>
     <t xml:space="preserve">other reasons </t>
+  </si>
+  <si>
+    <t>Serial_No</t>
+  </si>
+  <si>
+    <t>Name_of_Implementing__Partner</t>
+  </si>
+  <si>
+    <t>Implementing_Partner_Code</t>
+  </si>
+  <si>
+    <t>Dream_Client_FName</t>
+  </si>
+  <si>
+    <t>Dream_Client_MName</t>
+  </si>
+  <si>
+    <t>Dream_Client_LName</t>
+  </si>
+  <si>
+    <t>Date_of_Birth_</t>
+  </si>
+  <si>
+    <t>Client_Verification_Doc</t>
+  </si>
+  <si>
+    <t>Other_Specify</t>
+  </si>
+  <si>
+    <t>Identification_number_VER_Doc</t>
+  </si>
+  <si>
+    <t>Date_of_Enrollment</t>
+  </si>
+  <si>
+    <t>Month_of_Enrollment</t>
+  </si>
+  <si>
+    <t>Current_Age</t>
+  </si>
+  <si>
+    <t>Age_at_Enrollment</t>
+  </si>
+  <si>
+    <t>Marital_Status_client</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Ward_Code</t>
+  </si>
+  <si>
+    <t>Informal_settlement_Site</t>
+  </si>
+  <si>
+    <t>LandMark_Near_Residence</t>
+  </si>
+  <si>
+    <t>DREAMS_ID</t>
+  </si>
+  <si>
+    <t>DSS_ID</t>
+  </si>
+  <si>
+    <t>Name_of_primary_Fname</t>
+  </si>
+  <si>
+    <t>Name_of_primary_Mname</t>
+  </si>
+  <si>
+    <t>Name_of_primary_Lname</t>
+  </si>
+  <si>
+    <t>Rship_with_care_guardian</t>
+  </si>
+  <si>
+    <t>Specify_other_care_giver</t>
+  </si>
+  <si>
+    <t>P_Caregivers_Phone_No</t>
+  </si>
+  <si>
+    <t>NationalID_Passport_P_care_giver</t>
+  </si>
+  <si>
+    <t>Head_of_HH</t>
+  </si>
+  <si>
+    <t>Specify_other</t>
+  </si>
+  <si>
+    <t>Age_of_head_of_HH</t>
+  </si>
+  <si>
+    <t>Is_Father_Alive</t>
+  </si>
+  <si>
+    <t>Is_Mother_Alive_</t>
+  </si>
+  <si>
+    <t>Is_Parent_Guardian_Ill</t>
+  </si>
+  <si>
+    <t>floor_material</t>
+  </si>
+  <si>
+    <t>floor_Other_Specify</t>
+  </si>
+  <si>
+    <t>roof_material</t>
+  </si>
+  <si>
+    <t>roof_Other_Specify</t>
+  </si>
+  <si>
+    <t>wall_material</t>
+  </si>
+  <si>
+    <t>wall_material_Other_Specify</t>
+  </si>
+  <si>
+    <t>Mains_hsehold_H20</t>
+  </si>
+  <si>
+    <t>Mains_hsehold_H20_Other_Specify</t>
+  </si>
+  <si>
+    <t>Missed_food_last_month</t>
+  </si>
+  <si>
+    <t>How_Often</t>
+  </si>
+  <si>
+    <t>Any_form_of_disability</t>
+  </si>
+  <si>
+    <t>Hearing_impairment</t>
+  </si>
+  <si>
+    <t>Speech_impairment</t>
+  </si>
+  <si>
+    <t>Visual_impairment</t>
+  </si>
+  <si>
+    <t>Mental_impairment</t>
+  </si>
+  <si>
+    <t>Physical_impairment</t>
+  </si>
+  <si>
+    <t>other_Specify</t>
+  </si>
+  <si>
+    <t>Pple_living_in_the_Hsehold</t>
+  </si>
+  <si>
+    <t>EVER_enrolled_in_cash_transfer</t>
+  </si>
+  <si>
+    <t>Currently_enrolled_in_cash_transfer</t>
+  </si>
+  <si>
+    <t>Which_cash_transfer</t>
+  </si>
+  <si>
+    <t>Attending_school</t>
+  </si>
+  <si>
+    <t>Name_of_School</t>
+  </si>
+  <si>
+    <t>Type_of_School</t>
+  </si>
+  <si>
+    <t>Current_school_level</t>
+  </si>
+  <si>
+    <t>Class_Form</t>
+  </si>
+  <si>
+    <t>Government_bursary</t>
+  </si>
+  <si>
+    <t>Faith_Based</t>
+  </si>
+  <si>
+    <t>Main_reason_GIRL__not_in_school</t>
+  </si>
+  <si>
+    <t>Other_Specify_Girl_not_in_school</t>
+  </si>
+  <si>
+    <t>The_Last_time_in_school</t>
+  </si>
+  <si>
+    <t>Class_Form_stopped_schooling</t>
+  </si>
+  <si>
+    <t>Level_stopped_schooling</t>
+  </si>
+  <si>
+    <t>What_Girl_Wishes_to_do</t>
+  </si>
+  <si>
+    <t>Other_Specify_girl_wishes_to_do</t>
+  </si>
+  <si>
+    <t>Current_MAIN_source_of_income</t>
+  </si>
+  <si>
+    <t>Other_sources_of_income</t>
+  </si>
+  <si>
+    <t>Have_any_savings</t>
+  </si>
+  <si>
+    <t>Saving_Where</t>
+  </si>
+  <si>
+    <t>Other_Specify_Where_saving</t>
+  </si>
+  <si>
+    <t>Ever_been_tested_for_HIV</t>
+  </si>
+  <si>
+    <t>When_last_tested</t>
+  </si>
+  <si>
+    <t>Result_of_the_last_testing</t>
+  </si>
+  <si>
+    <t>If_HIV_Pos__currently_on_care</t>
+  </si>
+  <si>
+    <t>Seeking_HIV_care_at_which_facility</t>
+  </si>
+  <si>
+    <t>Main_reason_for_NOT_seeking_HIV_care</t>
+  </si>
+  <si>
+    <t>I_have_no_knowledge_about_HIV</t>
+  </si>
+  <si>
+    <t>I_don’t_know_where_to_get_one</t>
+  </si>
+  <si>
+    <t>I_cant_afford_it</t>
+  </si>
+  <si>
+    <t>Too_much_transport</t>
+  </si>
+  <si>
+    <t>Facility_is_far_away</t>
+  </si>
+  <si>
+    <t>I_am_afraid</t>
+  </si>
+  <si>
+    <t>I_don’t_need_to_test_Low_risk</t>
+  </si>
+  <si>
+    <t>Afraid_if_Ihave_HIV</t>
+  </si>
+  <si>
+    <t>Too_busy</t>
+  </si>
+  <si>
+    <t>Know_where_to_test</t>
+  </si>
+  <si>
+    <t>Ever_had_sex</t>
+  </si>
+  <si>
+    <t>Age_at_first_sex</t>
+  </si>
+  <si>
+    <t>no_sexual_partners_in_12_months</t>
+  </si>
+  <si>
+    <t>Do_you_have_current_sexual_partner</t>
+  </si>
+  <si>
+    <t>Age_of_Partner_Last_Sexual_partner</t>
+  </si>
+  <si>
+    <t>Age_of_Partner_Second_Last</t>
+  </si>
+  <si>
+    <t>Age_of_Partner_Third_Last</t>
+  </si>
+  <si>
+    <t>Partner_Circumcised_Last_Sexual_partner</t>
+  </si>
+  <si>
+    <t>Partner_Circumcised_Second_Last</t>
+  </si>
+  <si>
+    <t>Partner_Circumcised_Third_Last_partner</t>
+  </si>
+  <si>
+    <t>Knowledge_of_partners_HIV_status_Last_Sexual_partner</t>
+  </si>
+  <si>
+    <t>Knowledge_of_partners_HIV_status_Second_Last_partner</t>
+  </si>
+  <si>
+    <t>Knowledge_of_partners_HIV_status_Third_Last_Sexual_partner</t>
+  </si>
+  <si>
+    <t>Use_of_condom_with_Partner_Last_Sexual_partner</t>
+  </si>
+  <si>
+    <t>Ever_Received_gifts___favors_for_sex_last_12_months</t>
+  </si>
+  <si>
+    <t>Have_children</t>
+  </si>
+  <si>
+    <t>How_many_children</t>
+  </si>
+  <si>
+    <t>Currently_pregnant</t>
+  </si>
+  <si>
+    <t>Attending_ANC_clinic</t>
+  </si>
+  <si>
+    <t>Attending_ANC_Clinic_which_facility</t>
+  </si>
+  <si>
+    <t>Knowledge_of_FP_methods</t>
+  </si>
+  <si>
+    <t>Injectable</t>
+  </si>
+  <si>
+    <t>IUCD</t>
+  </si>
+  <si>
+    <t>other_FMP</t>
+  </si>
+  <si>
+    <t>Current_using_FP</t>
+  </si>
+  <si>
+    <t>Using_which_FP_Method</t>
+  </si>
+  <si>
+    <t>Using_which_FP_Other</t>
+  </si>
+  <si>
+    <t>Why_not_using_FP_Method</t>
+  </si>
+  <si>
+    <t>Why_not_using_FP_Method_Other</t>
+  </si>
+  <si>
+    <t>Said_or_did_something_to_humiliate_you_Ever</t>
+  </si>
+  <si>
+    <t>humiliate_you_Last_3_Months</t>
+  </si>
+  <si>
+    <t>Threat_close_to_girl_Ever</t>
+  </si>
+  <si>
+    <t>Threat_close_to_the_girl3_Months</t>
+  </si>
+  <si>
+    <t>Insult_or_made_you_feel_bad_Ever</t>
+  </si>
+  <si>
+    <t>Insult_feel_bad_Last_3_Months</t>
+  </si>
+  <si>
+    <t>Threat_your_economic_Ever</t>
+  </si>
+  <si>
+    <t>Threat_economic_3_Months</t>
+  </si>
+  <si>
+    <t>Pushed_Ever</t>
+  </si>
+  <si>
+    <t>Pushed_3_Months</t>
+  </si>
+  <si>
+    <t>forced_sex_Intercourse_Ever</t>
+  </si>
+  <si>
+    <t>forcesex_Intercourse_Last_3_Months</t>
+  </si>
+  <si>
+    <t>force_to_sex_acts_Ever</t>
+  </si>
+  <si>
+    <t>force_to_sex_acts_Last_3_Months</t>
+  </si>
+  <si>
+    <t>Force_threats_perform_acts_Ever</t>
+  </si>
+  <si>
+    <t>Force__perform_Last_3_Month</t>
+  </si>
+  <si>
+    <t>Sought_help_experiences</t>
+  </si>
+  <si>
+    <t>whom_whereseek_help_My_Family</t>
+  </si>
+  <si>
+    <t>whom_whereseek_help_Husband</t>
+  </si>
+  <si>
+    <t>whom_whereseek_help_Friend</t>
+  </si>
+  <si>
+    <t>whom_whereseek_help_Neighbour</t>
+  </si>
+  <si>
+    <t>whom_whereseek_help_Religious</t>
+  </si>
+  <si>
+    <t>whom_whereseek_help_med_personl</t>
+  </si>
+  <si>
+    <t>whom_whereseek_help_Chief</t>
+  </si>
+  <si>
+    <t>whom_whereseek_help_Police</t>
+  </si>
+  <si>
+    <t>whom_whereseek_help_Justice_sys</t>
+  </si>
+  <si>
+    <t>whom_whereseek_help_Ngo_CBO</t>
+  </si>
+  <si>
+    <t>whom_whereseek_help_Otr_spec</t>
+  </si>
+  <si>
+    <t>Know_where_to_seek_help</t>
+  </si>
+  <si>
+    <t>My_Family</t>
+  </si>
+  <si>
+    <t>Where_seek_help_Husband</t>
+  </si>
+  <si>
+    <t>Where_seek_help_Friend</t>
+  </si>
+  <si>
+    <t>Where_seek_help_Neighbour</t>
+  </si>
+  <si>
+    <t>Where_seek_help_Religious</t>
+  </si>
+  <si>
+    <t>Where_seek_help_med_perso</t>
+  </si>
+  <si>
+    <t>Where_seek_help_Chief</t>
+  </si>
+  <si>
+    <t>Where_seek_help_Police</t>
+  </si>
+  <si>
+    <t>Where_seek_help_Justice_sys</t>
+  </si>
+  <si>
+    <t>Where_seek_help_Ngo_CBO</t>
+  </si>
+  <si>
+    <t>Where_seek_help_Other</t>
+  </si>
+  <si>
+    <t>Used_alcohol_12Mon</t>
+  </si>
+  <si>
+    <t>Used_drug_past12Mon</t>
+  </si>
+  <si>
+    <t>type_drugs_12Months_Khat_Miraa</t>
+  </si>
+  <si>
+    <t>type_drugs_12Months_Glue_Gundi</t>
+  </si>
+  <si>
+    <t>type_drugs_12Months_Bhang</t>
+  </si>
+  <si>
+    <t>type_drugs_12Months_Cocaine</t>
+  </si>
+  <si>
+    <t>type_drugs_12Months_Heroin</t>
+  </si>
+  <si>
+    <t>type_drugs_12Months_Mandrax</t>
+  </si>
+  <si>
+    <t>type_drugs_12Months_Kuber</t>
+  </si>
+  <si>
+    <t>type_drugs_12Months_Tobacco</t>
+  </si>
+  <si>
+    <t>brew_sell_alcohol_12mon</t>
+  </si>
+  <si>
+    <t>HCBF</t>
+  </si>
+  <si>
+    <t>MHMC</t>
+  </si>
+  <si>
+    <t>Respect</t>
+  </si>
+  <si>
+    <t>SHUGA</t>
+  </si>
+  <si>
+    <t>SistertoSister</t>
+  </si>
+  <si>
+    <t>MLRC</t>
+  </si>
+  <si>
+    <t>FMP</t>
+  </si>
+  <si>
+    <t>None_inter</t>
+  </si>
+  <si>
+    <t>Other_inter</t>
+  </si>
+  <si>
+    <t>Howoften_past12Mon</t>
+  </si>
+  <si>
+    <t>type_drugs_12Months_other</t>
+  </si>
+  <si>
+    <t>Use_of_condom_with_Partner_Second_Last_Sexual_partner</t>
+  </si>
+  <si>
+    <t>Use_of_condom_with_Partner_Third_Last_Sexual_partner</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1569,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1126,6 +1676,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="7" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2421,7 +2974,7 @@
   </sheetPr>
   <dimension ref="A1:IU23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -2434,222 +2987,222 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:207" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="64"/>
-      <c r="R1" s="64"/>
-      <c r="S1" s="64"/>
-      <c r="T1" s="64"/>
-      <c r="U1" s="64"/>
-      <c r="V1" s="64"/>
-      <c r="W1" s="64"/>
-      <c r="X1" s="64"/>
-      <c r="Y1" s="64"/>
-      <c r="Z1" s="64"/>
-      <c r="AA1" s="64"/>
-      <c r="AB1" s="64"/>
-      <c r="AC1" s="64"/>
-      <c r="AD1" s="64"/>
-      <c r="AE1" s="64"/>
-      <c r="AF1" s="64"/>
-      <c r="AG1" s="64"/>
-      <c r="AH1" s="64"/>
-      <c r="AI1" s="64"/>
-      <c r="AJ1" s="64"/>
-      <c r="AK1" s="64"/>
-      <c r="AL1" s="64"/>
-      <c r="AM1" s="64"/>
-      <c r="AN1" s="64"/>
-      <c r="AO1" s="64"/>
-      <c r="AP1" s="64"/>
-      <c r="AQ1" s="64"/>
-      <c r="AR1" s="64"/>
-      <c r="AS1" s="64"/>
-      <c r="AT1" s="64"/>
-      <c r="AU1" s="64"/>
-      <c r="AV1" s="64"/>
-      <c r="AW1" s="64"/>
-      <c r="AX1" s="64"/>
-      <c r="AY1" s="64"/>
-      <c r="AZ1" s="64"/>
-      <c r="BA1" s="64"/>
-      <c r="BB1" s="64"/>
-      <c r="BC1" s="64"/>
-      <c r="BD1" s="64"/>
-      <c r="BE1" s="64"/>
-      <c r="BF1" s="64"/>
-      <c r="BG1" s="64"/>
-      <c r="BH1" s="64"/>
-      <c r="BI1" s="64"/>
-      <c r="BJ1" s="64"/>
-      <c r="BK1" s="64"/>
-      <c r="BL1" s="64"/>
-      <c r="BM1" s="64"/>
-      <c r="BN1" s="64"/>
-      <c r="BO1" s="64"/>
-      <c r="BP1" s="64"/>
-      <c r="BQ1" s="64"/>
-      <c r="BR1" s="64"/>
-      <c r="BS1" s="64"/>
-      <c r="BT1" s="64"/>
-      <c r="BU1" s="64"/>
-      <c r="BV1" s="64"/>
-      <c r="BW1" s="64"/>
-      <c r="BX1" s="64"/>
-      <c r="BY1" s="64"/>
-      <c r="BZ1" s="64"/>
-      <c r="CA1" s="64"/>
-      <c r="CB1" s="64"/>
-      <c r="CC1" s="64"/>
-      <c r="CD1" s="64"/>
-      <c r="CE1" s="64"/>
-      <c r="CF1" s="64"/>
-      <c r="CG1" s="64"/>
-      <c r="CH1" s="64"/>
-      <c r="CI1" s="64"/>
-      <c r="CJ1" s="64"/>
-      <c r="CK1" s="64"/>
-      <c r="CL1" s="64"/>
-      <c r="CM1" s="64"/>
-      <c r="CN1" s="64"/>
-      <c r="CO1" s="64"/>
-      <c r="CP1" s="64"/>
-      <c r="CQ1" s="64"/>
-      <c r="CR1" s="64"/>
-      <c r="CS1" s="64"/>
-      <c r="CT1" s="64"/>
-      <c r="CU1" s="64"/>
-      <c r="CV1" s="64"/>
-      <c r="CW1" s="64"/>
-      <c r="CX1" s="64"/>
-      <c r="CY1" s="64"/>
-      <c r="CZ1" s="64"/>
-      <c r="DA1" s="64"/>
-      <c r="DB1" s="64"/>
-      <c r="DC1" s="64"/>
-      <c r="DD1" s="64"/>
-      <c r="DE1" s="64"/>
-      <c r="DF1" s="64"/>
-      <c r="DG1" s="64"/>
-      <c r="DH1" s="64"/>
-      <c r="DI1" s="64"/>
-      <c r="DJ1" s="64"/>
-      <c r="DK1" s="64"/>
-      <c r="DL1" s="64"/>
-      <c r="DM1" s="64"/>
-      <c r="DN1" s="64"/>
-      <c r="DO1" s="64"/>
-      <c r="DP1" s="64"/>
-      <c r="DQ1" s="64"/>
-      <c r="DR1" s="64"/>
-      <c r="DS1" s="64"/>
-      <c r="DT1" s="64"/>
-      <c r="DU1" s="64"/>
-      <c r="DV1" s="64"/>
-      <c r="DW1" s="64"/>
-      <c r="DX1" s="64"/>
-      <c r="DY1" s="64"/>
-      <c r="DZ1" s="64"/>
-      <c r="EA1" s="64"/>
-      <c r="EB1" s="64"/>
-      <c r="EC1" s="64"/>
-      <c r="ED1" s="64"/>
-      <c r="EE1" s="64"/>
-      <c r="EF1" s="64"/>
-      <c r="EG1" s="64"/>
-      <c r="EH1" s="64"/>
-      <c r="EI1" s="64"/>
-      <c r="EJ1" s="64"/>
-      <c r="EK1" s="64"/>
-      <c r="EL1" s="64"/>
-      <c r="EM1" s="64"/>
-      <c r="EN1" s="64"/>
-      <c r="EO1" s="64"/>
-      <c r="EP1" s="64"/>
-      <c r="EQ1" s="64"/>
-      <c r="ER1" s="64"/>
-      <c r="ES1" s="64"/>
-      <c r="ET1" s="64"/>
-      <c r="EU1" s="64"/>
-      <c r="EV1" s="64"/>
-      <c r="EW1" s="64"/>
-      <c r="EX1" s="64"/>
-      <c r="EY1" s="64"/>
-      <c r="EZ1" s="64"/>
-      <c r="FA1" s="64"/>
-      <c r="FB1" s="64"/>
-      <c r="FC1" s="64"/>
-      <c r="FD1" s="64"/>
-      <c r="FE1" s="64"/>
-      <c r="FF1" s="64"/>
-      <c r="FG1" s="64"/>
-      <c r="FH1" s="64"/>
-      <c r="FI1" s="64"/>
-      <c r="FJ1" s="64"/>
-      <c r="FK1" s="64"/>
-      <c r="FL1" s="64"/>
-      <c r="FM1" s="64"/>
-      <c r="FN1" s="64"/>
-      <c r="FO1" s="64"/>
-      <c r="FP1" s="64"/>
-      <c r="FQ1" s="64"/>
-      <c r="FR1" s="64"/>
-      <c r="FS1" s="64"/>
-      <c r="FT1" s="64"/>
-      <c r="FU1" s="64"/>
-      <c r="FV1" s="64"/>
-      <c r="FW1" s="64"/>
-      <c r="FX1" s="64"/>
-      <c r="FY1" s="64"/>
-      <c r="FZ1" s="64"/>
-      <c r="GA1" s="64"/>
-      <c r="GB1" s="64"/>
-      <c r="GC1" s="64"/>
-      <c r="GD1" s="64"/>
-      <c r="GE1" s="64"/>
-      <c r="GF1" s="64"/>
-      <c r="GG1" s="64"/>
-      <c r="GH1" s="64"/>
-      <c r="GI1" s="64"/>
-      <c r="GJ1" s="64"/>
-      <c r="GK1" s="64"/>
-      <c r="GL1" s="64"/>
-      <c r="GM1" s="64"/>
-      <c r="GN1" s="64"/>
-      <c r="GO1" s="64"/>
-      <c r="GP1" s="64"/>
-      <c r="GQ1" s="64"/>
-      <c r="GR1" s="64"/>
-      <c r="GS1" s="64"/>
-      <c r="GT1" s="64"/>
-      <c r="GU1" s="64"/>
-      <c r="GV1" s="64"/>
-      <c r="GW1" s="64"/>
-      <c r="GX1" s="64"/>
-      <c r="GY1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65"/>
+      <c r="AF1" s="65"/>
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65"/>
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="65"/>
+      <c r="AK1" s="65"/>
+      <c r="AL1" s="65"/>
+      <c r="AM1" s="65"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="65"/>
+      <c r="AP1" s="65"/>
+      <c r="AQ1" s="65"/>
+      <c r="AR1" s="65"/>
+      <c r="AS1" s="65"/>
+      <c r="AT1" s="65"/>
+      <c r="AU1" s="65"/>
+      <c r="AV1" s="65"/>
+      <c r="AW1" s="65"/>
+      <c r="AX1" s="65"/>
+      <c r="AY1" s="65"/>
+      <c r="AZ1" s="65"/>
+      <c r="BA1" s="65"/>
+      <c r="BB1" s="65"/>
+      <c r="BC1" s="65"/>
+      <c r="BD1" s="65"/>
+      <c r="BE1" s="65"/>
+      <c r="BF1" s="65"/>
+      <c r="BG1" s="65"/>
+      <c r="BH1" s="65"/>
+      <c r="BI1" s="65"/>
+      <c r="BJ1" s="65"/>
+      <c r="BK1" s="65"/>
+      <c r="BL1" s="65"/>
+      <c r="BM1" s="65"/>
+      <c r="BN1" s="65"/>
+      <c r="BO1" s="65"/>
+      <c r="BP1" s="65"/>
+      <c r="BQ1" s="65"/>
+      <c r="BR1" s="65"/>
+      <c r="BS1" s="65"/>
+      <c r="BT1" s="65"/>
+      <c r="BU1" s="65"/>
+      <c r="BV1" s="65"/>
+      <c r="BW1" s="65"/>
+      <c r="BX1" s="65"/>
+      <c r="BY1" s="65"/>
+      <c r="BZ1" s="65"/>
+      <c r="CA1" s="65"/>
+      <c r="CB1" s="65"/>
+      <c r="CC1" s="65"/>
+      <c r="CD1" s="65"/>
+      <c r="CE1" s="65"/>
+      <c r="CF1" s="65"/>
+      <c r="CG1" s="65"/>
+      <c r="CH1" s="65"/>
+      <c r="CI1" s="65"/>
+      <c r="CJ1" s="65"/>
+      <c r="CK1" s="65"/>
+      <c r="CL1" s="65"/>
+      <c r="CM1" s="65"/>
+      <c r="CN1" s="65"/>
+      <c r="CO1" s="65"/>
+      <c r="CP1" s="65"/>
+      <c r="CQ1" s="65"/>
+      <c r="CR1" s="65"/>
+      <c r="CS1" s="65"/>
+      <c r="CT1" s="65"/>
+      <c r="CU1" s="65"/>
+      <c r="CV1" s="65"/>
+      <c r="CW1" s="65"/>
+      <c r="CX1" s="65"/>
+      <c r="CY1" s="65"/>
+      <c r="CZ1" s="65"/>
+      <c r="DA1" s="65"/>
+      <c r="DB1" s="65"/>
+      <c r="DC1" s="65"/>
+      <c r="DD1" s="65"/>
+      <c r="DE1" s="65"/>
+      <c r="DF1" s="65"/>
+      <c r="DG1" s="65"/>
+      <c r="DH1" s="65"/>
+      <c r="DI1" s="65"/>
+      <c r="DJ1" s="65"/>
+      <c r="DK1" s="65"/>
+      <c r="DL1" s="65"/>
+      <c r="DM1" s="65"/>
+      <c r="DN1" s="65"/>
+      <c r="DO1" s="65"/>
+      <c r="DP1" s="65"/>
+      <c r="DQ1" s="65"/>
+      <c r="DR1" s="65"/>
+      <c r="DS1" s="65"/>
+      <c r="DT1" s="65"/>
+      <c r="DU1" s="65"/>
+      <c r="DV1" s="65"/>
+      <c r="DW1" s="65"/>
+      <c r="DX1" s="65"/>
+      <c r="DY1" s="65"/>
+      <c r="DZ1" s="65"/>
+      <c r="EA1" s="65"/>
+      <c r="EB1" s="65"/>
+      <c r="EC1" s="65"/>
+      <c r="ED1" s="65"/>
+      <c r="EE1" s="65"/>
+      <c r="EF1" s="65"/>
+      <c r="EG1" s="65"/>
+      <c r="EH1" s="65"/>
+      <c r="EI1" s="65"/>
+      <c r="EJ1" s="65"/>
+      <c r="EK1" s="65"/>
+      <c r="EL1" s="65"/>
+      <c r="EM1" s="65"/>
+      <c r="EN1" s="65"/>
+      <c r="EO1" s="65"/>
+      <c r="EP1" s="65"/>
+      <c r="EQ1" s="65"/>
+      <c r="ER1" s="65"/>
+      <c r="ES1" s="65"/>
+      <c r="ET1" s="65"/>
+      <c r="EU1" s="65"/>
+      <c r="EV1" s="65"/>
+      <c r="EW1" s="65"/>
+      <c r="EX1" s="65"/>
+      <c r="EY1" s="65"/>
+      <c r="EZ1" s="65"/>
+      <c r="FA1" s="65"/>
+      <c r="FB1" s="65"/>
+      <c r="FC1" s="65"/>
+      <c r="FD1" s="65"/>
+      <c r="FE1" s="65"/>
+      <c r="FF1" s="65"/>
+      <c r="FG1" s="65"/>
+      <c r="FH1" s="65"/>
+      <c r="FI1" s="65"/>
+      <c r="FJ1" s="65"/>
+      <c r="FK1" s="65"/>
+      <c r="FL1" s="65"/>
+      <c r="FM1" s="65"/>
+      <c r="FN1" s="65"/>
+      <c r="FO1" s="65"/>
+      <c r="FP1" s="65"/>
+      <c r="FQ1" s="65"/>
+      <c r="FR1" s="65"/>
+      <c r="FS1" s="65"/>
+      <c r="FT1" s="65"/>
+      <c r="FU1" s="65"/>
+      <c r="FV1" s="65"/>
+      <c r="FW1" s="65"/>
+      <c r="FX1" s="65"/>
+      <c r="FY1" s="65"/>
+      <c r="FZ1" s="65"/>
+      <c r="GA1" s="65"/>
+      <c r="GB1" s="65"/>
+      <c r="GC1" s="65"/>
+      <c r="GD1" s="65"/>
+      <c r="GE1" s="65"/>
+      <c r="GF1" s="65"/>
+      <c r="GG1" s="65"/>
+      <c r="GH1" s="65"/>
+      <c r="GI1" s="65"/>
+      <c r="GJ1" s="65"/>
+      <c r="GK1" s="65"/>
+      <c r="GL1" s="65"/>
+      <c r="GM1" s="65"/>
+      <c r="GN1" s="65"/>
+      <c r="GO1" s="65"/>
+      <c r="GP1" s="65"/>
+      <c r="GQ1" s="65"/>
+      <c r="GR1" s="65"/>
+      <c r="GS1" s="65"/>
+      <c r="GT1" s="65"/>
+      <c r="GU1" s="65"/>
+      <c r="GV1" s="65"/>
+      <c r="GW1" s="65"/>
+      <c r="GX1" s="65"/>
+      <c r="GY1" s="65"/>
     </row>
     <row r="2" spans="1:207" ht="36.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2680,628 +3233,628 @@
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
       <c r="AE2" s="4"/>
-      <c r="AF2" s="53" t="s">
+      <c r="AF2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="AG2" s="54"/>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54"/>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
-      <c r="AM2" s="54"/>
-      <c r="AN2" s="54"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="54"/>
-      <c r="AQ2" s="54"/>
-      <c r="AR2" s="54"/>
-      <c r="AS2" s="54"/>
-      <c r="AT2" s="54"/>
-      <c r="AU2" s="54"/>
-      <c r="AV2" s="54"/>
-      <c r="AW2" s="54"/>
-      <c r="AX2" s="54"/>
-      <c r="AY2" s="54"/>
-      <c r="AZ2" s="54"/>
-      <c r="BA2" s="54"/>
-      <c r="BB2" s="54"/>
-      <c r="BC2" s="54"/>
-      <c r="BD2" s="54"/>
-      <c r="BE2" s="54"/>
-      <c r="BF2" s="54"/>
-      <c r="BG2" s="54"/>
-      <c r="BH2" s="54"/>
-      <c r="BI2" s="54"/>
-      <c r="BJ2" s="55"/>
-      <c r="BK2" s="56" t="s">
+      <c r="AG2" s="55"/>
+      <c r="AH2" s="55"/>
+      <c r="AI2" s="55"/>
+      <c r="AJ2" s="55"/>
+      <c r="AK2" s="55"/>
+      <c r="AL2" s="55"/>
+      <c r="AM2" s="55"/>
+      <c r="AN2" s="55"/>
+      <c r="AO2" s="55"/>
+      <c r="AP2" s="55"/>
+      <c r="AQ2" s="55"/>
+      <c r="AR2" s="55"/>
+      <c r="AS2" s="55"/>
+      <c r="AT2" s="55"/>
+      <c r="AU2" s="55"/>
+      <c r="AV2" s="55"/>
+      <c r="AW2" s="55"/>
+      <c r="AX2" s="55"/>
+      <c r="AY2" s="55"/>
+      <c r="AZ2" s="55"/>
+      <c r="BA2" s="55"/>
+      <c r="BB2" s="55"/>
+      <c r="BC2" s="55"/>
+      <c r="BD2" s="55"/>
+      <c r="BE2" s="55"/>
+      <c r="BF2" s="55"/>
+      <c r="BG2" s="55"/>
+      <c r="BH2" s="55"/>
+      <c r="BI2" s="55"/>
+      <c r="BJ2" s="56"/>
+      <c r="BK2" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="BL2" s="57"/>
-      <c r="BM2" s="57"/>
-      <c r="BN2" s="57"/>
-      <c r="BO2" s="57"/>
-      <c r="BP2" s="57"/>
-      <c r="BQ2" s="57"/>
-      <c r="BR2" s="57"/>
-      <c r="BS2" s="57"/>
-      <c r="BT2" s="57"/>
-      <c r="BU2" s="57"/>
-      <c r="BV2" s="57"/>
-      <c r="BW2" s="57"/>
-      <c r="BX2" s="57"/>
-      <c r="BY2" s="57"/>
-      <c r="BZ2" s="57"/>
-      <c r="CA2" s="57"/>
-      <c r="CB2" s="57"/>
-      <c r="CC2" s="57"/>
-      <c r="CD2" s="57"/>
-      <c r="CE2" s="57"/>
-      <c r="CF2" s="57"/>
-      <c r="CG2" s="57"/>
-      <c r="CH2" s="58"/>
-      <c r="CI2" s="41" t="s">
+      <c r="BL2" s="58"/>
+      <c r="BM2" s="58"/>
+      <c r="BN2" s="58"/>
+      <c r="BO2" s="58"/>
+      <c r="BP2" s="58"/>
+      <c r="BQ2" s="58"/>
+      <c r="BR2" s="58"/>
+      <c r="BS2" s="58"/>
+      <c r="BT2" s="58"/>
+      <c r="BU2" s="58"/>
+      <c r="BV2" s="58"/>
+      <c r="BW2" s="58"/>
+      <c r="BX2" s="58"/>
+      <c r="BY2" s="58"/>
+      <c r="BZ2" s="58"/>
+      <c r="CA2" s="58"/>
+      <c r="CB2" s="58"/>
+      <c r="CC2" s="58"/>
+      <c r="CD2" s="58"/>
+      <c r="CE2" s="58"/>
+      <c r="CF2" s="58"/>
+      <c r="CG2" s="58"/>
+      <c r="CH2" s="59"/>
+      <c r="CI2" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="CJ2" s="42"/>
-      <c r="CK2" s="42"/>
-      <c r="CL2" s="42"/>
-      <c r="CM2" s="42"/>
-      <c r="CN2" s="42"/>
-      <c r="CO2" s="42"/>
-      <c r="CP2" s="42"/>
-      <c r="CQ2" s="42"/>
-      <c r="CR2" s="42"/>
-      <c r="CS2" s="42"/>
-      <c r="CT2" s="42"/>
-      <c r="CU2" s="42"/>
-      <c r="CV2" s="42"/>
-      <c r="CW2" s="42"/>
-      <c r="CX2" s="42"/>
-      <c r="CY2" s="42"/>
-      <c r="CZ2" s="43"/>
-      <c r="DA2" s="46" t="s">
+      <c r="CJ2" s="43"/>
+      <c r="CK2" s="43"/>
+      <c r="CL2" s="43"/>
+      <c r="CM2" s="43"/>
+      <c r="CN2" s="43"/>
+      <c r="CO2" s="43"/>
+      <c r="CP2" s="43"/>
+      <c r="CQ2" s="43"/>
+      <c r="CR2" s="43"/>
+      <c r="CS2" s="43"/>
+      <c r="CT2" s="43"/>
+      <c r="CU2" s="43"/>
+      <c r="CV2" s="43"/>
+      <c r="CW2" s="43"/>
+      <c r="CX2" s="43"/>
+      <c r="CY2" s="43"/>
+      <c r="CZ2" s="44"/>
+      <c r="DA2" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="DB2" s="47"/>
-      <c r="DC2" s="47"/>
-      <c r="DD2" s="47"/>
-      <c r="DE2" s="47"/>
-      <c r="DF2" s="47"/>
-      <c r="DG2" s="47"/>
-      <c r="DH2" s="47"/>
-      <c r="DI2" s="47"/>
-      <c r="DJ2" s="47"/>
-      <c r="DK2" s="47"/>
-      <c r="DL2" s="47"/>
-      <c r="DM2" s="47"/>
-      <c r="DN2" s="47"/>
-      <c r="DO2" s="47"/>
-      <c r="DP2" s="47"/>
-      <c r="DQ2" s="48"/>
-      <c r="DR2" s="38" t="s">
+      <c r="DB2" s="48"/>
+      <c r="DC2" s="48"/>
+      <c r="DD2" s="48"/>
+      <c r="DE2" s="48"/>
+      <c r="DF2" s="48"/>
+      <c r="DG2" s="48"/>
+      <c r="DH2" s="48"/>
+      <c r="DI2" s="48"/>
+      <c r="DJ2" s="48"/>
+      <c r="DK2" s="48"/>
+      <c r="DL2" s="48"/>
+      <c r="DM2" s="48"/>
+      <c r="DN2" s="48"/>
+      <c r="DO2" s="48"/>
+      <c r="DP2" s="48"/>
+      <c r="DQ2" s="49"/>
+      <c r="DR2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="DS2" s="39"/>
-      <c r="DT2" s="39"/>
-      <c r="DU2" s="39"/>
-      <c r="DV2" s="39"/>
-      <c r="DW2" s="39"/>
-      <c r="DX2" s="39"/>
-      <c r="DY2" s="39"/>
-      <c r="DZ2" s="39"/>
-      <c r="EA2" s="39"/>
-      <c r="EB2" s="39"/>
-      <c r="EC2" s="39"/>
-      <c r="ED2" s="39"/>
-      <c r="EE2" s="39"/>
-      <c r="EF2" s="39"/>
-      <c r="EG2" s="39"/>
-      <c r="EH2" s="39"/>
-      <c r="EI2" s="40"/>
-      <c r="EJ2" s="41" t="s">
+      <c r="DS2" s="40"/>
+      <c r="DT2" s="40"/>
+      <c r="DU2" s="40"/>
+      <c r="DV2" s="40"/>
+      <c r="DW2" s="40"/>
+      <c r="DX2" s="40"/>
+      <c r="DY2" s="40"/>
+      <c r="DZ2" s="40"/>
+      <c r="EA2" s="40"/>
+      <c r="EB2" s="40"/>
+      <c r="EC2" s="40"/>
+      <c r="ED2" s="40"/>
+      <c r="EE2" s="40"/>
+      <c r="EF2" s="40"/>
+      <c r="EG2" s="40"/>
+      <c r="EH2" s="40"/>
+      <c r="EI2" s="41"/>
+      <c r="EJ2" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="EK2" s="42"/>
-      <c r="EL2" s="42"/>
-      <c r="EM2" s="42"/>
-      <c r="EN2" s="42"/>
-      <c r="EO2" s="42"/>
-      <c r="EP2" s="42"/>
-      <c r="EQ2" s="42"/>
-      <c r="ER2" s="42"/>
-      <c r="ES2" s="42"/>
-      <c r="ET2" s="42"/>
-      <c r="EU2" s="42"/>
-      <c r="EV2" s="42"/>
-      <c r="EW2" s="42"/>
-      <c r="EX2" s="42"/>
-      <c r="EY2" s="42"/>
-      <c r="EZ2" s="42"/>
-      <c r="FA2" s="42"/>
-      <c r="FB2" s="42"/>
-      <c r="FC2" s="42"/>
-      <c r="FD2" s="42"/>
-      <c r="FE2" s="42"/>
-      <c r="FF2" s="42"/>
-      <c r="FG2" s="42"/>
-      <c r="FH2" s="42"/>
-      <c r="FI2" s="42"/>
-      <c r="FJ2" s="42"/>
-      <c r="FK2" s="42"/>
-      <c r="FL2" s="42"/>
-      <c r="FM2" s="42"/>
-      <c r="FN2" s="42"/>
-      <c r="FO2" s="42"/>
-      <c r="FP2" s="42"/>
-      <c r="FQ2" s="42"/>
-      <c r="FR2" s="42"/>
-      <c r="FS2" s="42"/>
-      <c r="FT2" s="42"/>
-      <c r="FU2" s="42"/>
-      <c r="FV2" s="42"/>
-      <c r="FW2" s="43"/>
-      <c r="FX2" s="46" t="s">
+      <c r="EK2" s="43"/>
+      <c r="EL2" s="43"/>
+      <c r="EM2" s="43"/>
+      <c r="EN2" s="43"/>
+      <c r="EO2" s="43"/>
+      <c r="EP2" s="43"/>
+      <c r="EQ2" s="43"/>
+      <c r="ER2" s="43"/>
+      <c r="ES2" s="43"/>
+      <c r="ET2" s="43"/>
+      <c r="EU2" s="43"/>
+      <c r="EV2" s="43"/>
+      <c r="EW2" s="43"/>
+      <c r="EX2" s="43"/>
+      <c r="EY2" s="43"/>
+      <c r="EZ2" s="43"/>
+      <c r="FA2" s="43"/>
+      <c r="FB2" s="43"/>
+      <c r="FC2" s="43"/>
+      <c r="FD2" s="43"/>
+      <c r="FE2" s="43"/>
+      <c r="FF2" s="43"/>
+      <c r="FG2" s="43"/>
+      <c r="FH2" s="43"/>
+      <c r="FI2" s="43"/>
+      <c r="FJ2" s="43"/>
+      <c r="FK2" s="43"/>
+      <c r="FL2" s="43"/>
+      <c r="FM2" s="43"/>
+      <c r="FN2" s="43"/>
+      <c r="FO2" s="43"/>
+      <c r="FP2" s="43"/>
+      <c r="FQ2" s="43"/>
+      <c r="FR2" s="43"/>
+      <c r="FS2" s="43"/>
+      <c r="FT2" s="43"/>
+      <c r="FU2" s="43"/>
+      <c r="FV2" s="43"/>
+      <c r="FW2" s="44"/>
+      <c r="FX2" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="FY2" s="47"/>
-      <c r="FZ2" s="47"/>
-      <c r="GA2" s="47"/>
-      <c r="GB2" s="47"/>
-      <c r="GC2" s="47"/>
-      <c r="GD2" s="47"/>
-      <c r="GE2" s="47"/>
-      <c r="GF2" s="47"/>
-      <c r="GG2" s="47"/>
-      <c r="GH2" s="47"/>
-      <c r="GI2" s="47"/>
-      <c r="GJ2" s="48"/>
-      <c r="GK2" s="38" t="s">
+      <c r="FY2" s="48"/>
+      <c r="FZ2" s="48"/>
+      <c r="GA2" s="48"/>
+      <c r="GB2" s="48"/>
+      <c r="GC2" s="48"/>
+      <c r="GD2" s="48"/>
+      <c r="GE2" s="48"/>
+      <c r="GF2" s="48"/>
+      <c r="GG2" s="48"/>
+      <c r="GH2" s="48"/>
+      <c r="GI2" s="48"/>
+      <c r="GJ2" s="49"/>
+      <c r="GK2" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="GL2" s="39"/>
-      <c r="GM2" s="39"/>
-      <c r="GN2" s="39"/>
-      <c r="GO2" s="39"/>
-      <c r="GP2" s="39"/>
-      <c r="GQ2" s="39"/>
-      <c r="GR2" s="39"/>
-      <c r="GS2" s="40"/>
+      <c r="GL2" s="40"/>
+      <c r="GM2" s="40"/>
+      <c r="GN2" s="40"/>
+      <c r="GO2" s="40"/>
+      <c r="GP2" s="40"/>
+      <c r="GQ2" s="40"/>
+      <c r="GR2" s="40"/>
+      <c r="GS2" s="41"/>
       <c r="GT2" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="GU2" s="62" t="s">
+      <c r="GU2" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="GV2" s="63"/>
-      <c r="GW2" s="63"/>
+      <c r="GV2" s="64"/>
+      <c r="GW2" s="64"/>
       <c r="GX2" s="5"/>
       <c r="GY2" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:207" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="36" t="s">
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="36" t="s">
+      <c r="K3" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="36" t="s">
+      <c r="L3" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="36" t="s">
+      <c r="M3" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="36" t="s">
+      <c r="N3" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="36" t="s">
+      <c r="O3" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="36" t="s">
+      <c r="P3" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="36" t="s">
+      <c r="Q3" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="36" t="s">
+      <c r="R3" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="S3" s="36" t="s">
+      <c r="S3" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="T3" s="36" t="s">
+      <c r="T3" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="U3" s="36" t="s">
+      <c r="U3" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="V3" s="36" t="s">
+      <c r="V3" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="W3" s="36" t="s">
+      <c r="W3" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="X3" s="36" t="s">
+      <c r="X3" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="Y3" s="36" t="s">
+      <c r="Y3" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="36" t="s">
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="AC3" s="37"/>
-      <c r="AD3" s="36" t="s">
+      <c r="AC3" s="38"/>
+      <c r="AD3" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="AE3" s="36" t="s">
+      <c r="AE3" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="AF3" s="36" t="s">
+      <c r="AF3" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="AG3" s="37"/>
-      <c r="AH3" s="36" t="s">
+      <c r="AG3" s="38"/>
+      <c r="AH3" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="AI3" s="36" t="s">
+      <c r="AI3" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="AJ3" s="36" t="s">
+      <c r="AJ3" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="AK3" s="36" t="s">
+      <c r="AK3" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="AL3" s="36" t="s">
+      <c r="AL3" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="AM3" s="37"/>
-      <c r="AN3" s="36" t="s">
+      <c r="AM3" s="38"/>
+      <c r="AN3" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="AO3" s="37"/>
-      <c r="AP3" s="36" t="s">
+      <c r="AO3" s="38"/>
+      <c r="AP3" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="AQ3" s="37"/>
-      <c r="AR3" s="36" t="s">
+      <c r="AQ3" s="38"/>
+      <c r="AR3" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="AS3" s="37"/>
-      <c r="AT3" s="36" t="s">
+      <c r="AS3" s="38"/>
+      <c r="AT3" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="AU3" s="36" t="s">
+      <c r="AU3" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="AV3" s="36" t="s">
+      <c r="AV3" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="AW3" s="36" t="s">
+      <c r="AW3" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="AX3" s="37"/>
-      <c r="AY3" s="37"/>
-      <c r="AZ3" s="37"/>
-      <c r="BA3" s="37"/>
-      <c r="BB3" s="37"/>
-      <c r="BC3" s="36" t="s">
+      <c r="AX3" s="38"/>
+      <c r="AY3" s="38"/>
+      <c r="AZ3" s="38"/>
+      <c r="BA3" s="38"/>
+      <c r="BB3" s="38"/>
+      <c r="BC3" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="BD3" s="36" t="s">
+      <c r="BD3" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="BE3" s="36" t="s">
+      <c r="BE3" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="BF3" s="36" t="s">
+      <c r="BF3" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="BG3" s="36" t="s">
+      <c r="BG3" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="BH3" s="36" t="s">
+      <c r="BH3" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="BI3" s="37"/>
-      <c r="BJ3" s="37"/>
-      <c r="BK3" s="36" t="s">
+      <c r="BI3" s="38"/>
+      <c r="BJ3" s="38"/>
+      <c r="BK3" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="BL3" s="36" t="s">
+      <c r="BL3" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="BM3" s="37"/>
-      <c r="BN3" s="36" t="s">
+      <c r="BM3" s="38"/>
+      <c r="BN3" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="BO3" s="37"/>
-      <c r="BP3" s="37"/>
-      <c r="BQ3" s="36" t="s">
+      <c r="BO3" s="38"/>
+      <c r="BP3" s="38"/>
+      <c r="BQ3" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="BR3" s="37"/>
-      <c r="BS3" s="37"/>
-      <c r="BT3" s="37"/>
-      <c r="BU3" s="37"/>
-      <c r="BV3" s="37"/>
-      <c r="BW3" s="36" t="s">
+      <c r="BR3" s="38"/>
+      <c r="BS3" s="38"/>
+      <c r="BT3" s="38"/>
+      <c r="BU3" s="38"/>
+      <c r="BV3" s="38"/>
+      <c r="BW3" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="BX3" s="37"/>
-      <c r="BY3" s="36" t="s">
+      <c r="BX3" s="38"/>
+      <c r="BY3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="BZ3" s="36" t="s">
+      <c r="BZ3" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="CA3" s="37"/>
-      <c r="CB3" s="36" t="s">
+      <c r="CA3" s="38"/>
+      <c r="CB3" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="CC3" s="37"/>
-      <c r="CD3" s="36" t="s">
+      <c r="CC3" s="38"/>
+      <c r="CD3" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="CE3" s="37"/>
+      <c r="CE3" s="38"/>
       <c r="CF3" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="CG3" s="36" t="s">
+      <c r="CG3" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="CH3" s="37"/>
-      <c r="CI3" s="36" t="s">
+      <c r="CH3" s="38"/>
+      <c r="CI3" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="CJ3" s="36" t="s">
+      <c r="CJ3" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="CK3" s="36" t="s">
+      <c r="CK3" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="CL3" s="36" t="s">
+      <c r="CL3" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="CM3" s="36" t="s">
+      <c r="CM3" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="CN3" s="36" t="s">
+      <c r="CN3" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="CO3" s="36" t="s">
+      <c r="CO3" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="CP3" s="36" t="s">
+      <c r="CP3" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="CQ3" s="37"/>
-      <c r="CR3" s="37"/>
-      <c r="CS3" s="37"/>
-      <c r="CT3" s="37"/>
-      <c r="CU3" s="37"/>
-      <c r="CV3" s="37"/>
-      <c r="CW3" s="37"/>
-      <c r="CX3" s="37"/>
-      <c r="CY3" s="37"/>
-      <c r="CZ3" s="36" t="s">
+      <c r="CQ3" s="38"/>
+      <c r="CR3" s="38"/>
+      <c r="CS3" s="38"/>
+      <c r="CT3" s="38"/>
+      <c r="CU3" s="38"/>
+      <c r="CV3" s="38"/>
+      <c r="CW3" s="38"/>
+      <c r="CX3" s="38"/>
+      <c r="CY3" s="38"/>
+      <c r="CZ3" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="DA3" s="36" t="s">
+      <c r="DA3" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="DB3" s="36" t="s">
+      <c r="DB3" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="DC3" s="36" t="s">
+      <c r="DC3" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="DD3" s="36" t="s">
+      <c r="DD3" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="DE3" s="36" t="s">
+      <c r="DE3" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="DF3" s="37"/>
-      <c r="DG3" s="37"/>
-      <c r="DH3" s="36" t="s">
+      <c r="DF3" s="38"/>
+      <c r="DG3" s="38"/>
+      <c r="DH3" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="DI3" s="37"/>
-      <c r="DJ3" s="37"/>
-      <c r="DK3" s="36" t="s">
+      <c r="DI3" s="38"/>
+      <c r="DJ3" s="38"/>
+      <c r="DK3" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="DL3" s="37"/>
-      <c r="DM3" s="37"/>
-      <c r="DN3" s="36" t="s">
+      <c r="DL3" s="38"/>
+      <c r="DM3" s="38"/>
+      <c r="DN3" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="DO3" s="37"/>
-      <c r="DP3" s="37"/>
-      <c r="DQ3" s="36" t="s">
+      <c r="DO3" s="38"/>
+      <c r="DP3" s="38"/>
+      <c r="DQ3" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="DR3" s="36" t="s">
+      <c r="DR3" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="DS3" s="36" t="s">
+      <c r="DS3" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="DT3" s="36" t="s">
+      <c r="DT3" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="DU3" s="36" t="s">
+      <c r="DU3" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="DV3" s="36" t="s">
+      <c r="DV3" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="DW3" s="36" t="s">
+      <c r="DW3" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="DX3" s="36" t="s">
+      <c r="DX3" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="DY3" s="37"/>
-      <c r="DZ3" s="37"/>
-      <c r="EA3" s="37"/>
-      <c r="EB3" s="37"/>
-      <c r="EC3" s="37"/>
-      <c r="ED3" s="37"/>
-      <c r="EE3" s="36" t="s">
+      <c r="DY3" s="38"/>
+      <c r="DZ3" s="38"/>
+      <c r="EA3" s="38"/>
+      <c r="EB3" s="38"/>
+      <c r="EC3" s="38"/>
+      <c r="ED3" s="38"/>
+      <c r="EE3" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="EF3" s="36" t="s">
+      <c r="EF3" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="EG3" s="37"/>
-      <c r="EH3" s="36" t="s">
+      <c r="EG3" s="38"/>
+      <c r="EH3" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="EI3" s="37"/>
-      <c r="EJ3" s="36" t="s">
+      <c r="EI3" s="38"/>
+      <c r="EJ3" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="EK3" s="37"/>
-      <c r="EL3" s="36" t="s">
+      <c r="EK3" s="38"/>
+      <c r="EL3" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="EM3" s="37"/>
-      <c r="EN3" s="36" t="s">
+      <c r="EM3" s="38"/>
+      <c r="EN3" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="EO3" s="37"/>
-      <c r="EP3" s="36" t="s">
+      <c r="EO3" s="38"/>
+      <c r="EP3" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="EQ3" s="37"/>
-      <c r="ER3" s="36" t="s">
+      <c r="EQ3" s="38"/>
+      <c r="ER3" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="ES3" s="37"/>
-      <c r="ET3" s="36" t="s">
+      <c r="ES3" s="38"/>
+      <c r="ET3" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="EU3" s="37"/>
-      <c r="EV3" s="36" t="s">
+      <c r="EU3" s="38"/>
+      <c r="EV3" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="EW3" s="37"/>
-      <c r="EX3" s="36" t="s">
+      <c r="EW3" s="38"/>
+      <c r="EX3" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="EY3" s="37"/>
-      <c r="EZ3" s="36" t="s">
+      <c r="EY3" s="38"/>
+      <c r="EZ3" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="FA3" s="36" t="s">
+      <c r="FA3" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="FB3" s="37"/>
-      <c r="FC3" s="37"/>
-      <c r="FD3" s="37"/>
-      <c r="FE3" s="37"/>
-      <c r="FF3" s="37"/>
-      <c r="FG3" s="37"/>
-      <c r="FH3" s="37"/>
-      <c r="FI3" s="37"/>
-      <c r="FJ3" s="37"/>
-      <c r="FK3" s="37"/>
-      <c r="FL3" s="36" t="s">
+      <c r="FB3" s="38"/>
+      <c r="FC3" s="38"/>
+      <c r="FD3" s="38"/>
+      <c r="FE3" s="38"/>
+      <c r="FF3" s="38"/>
+      <c r="FG3" s="38"/>
+      <c r="FH3" s="38"/>
+      <c r="FI3" s="38"/>
+      <c r="FJ3" s="38"/>
+      <c r="FK3" s="38"/>
+      <c r="FL3" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="FM3" s="36" t="s">
+      <c r="FM3" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="FN3" s="37"/>
-      <c r="FO3" s="37"/>
-      <c r="FP3" s="37"/>
-      <c r="FQ3" s="37"/>
-      <c r="FR3" s="37"/>
-      <c r="FS3" s="37"/>
-      <c r="FT3" s="37"/>
-      <c r="FU3" s="37"/>
-      <c r="FV3" s="37"/>
-      <c r="FW3" s="37"/>
-      <c r="FX3" s="36" t="s">
+      <c r="FN3" s="38"/>
+      <c r="FO3" s="38"/>
+      <c r="FP3" s="38"/>
+      <c r="FQ3" s="38"/>
+      <c r="FR3" s="38"/>
+      <c r="FS3" s="38"/>
+      <c r="FT3" s="38"/>
+      <c r="FU3" s="38"/>
+      <c r="FV3" s="38"/>
+      <c r="FW3" s="38"/>
+      <c r="FX3" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="FY3" s="36" t="s">
+      <c r="FY3" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="FZ3" s="36" t="s">
+      <c r="FZ3" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="GA3" s="44" t="s">
+      <c r="GA3" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="GB3" s="45"/>
-      <c r="GC3" s="45"/>
-      <c r="GD3" s="45"/>
-      <c r="GE3" s="45"/>
-      <c r="GF3" s="45"/>
-      <c r="GG3" s="45"/>
-      <c r="GH3" s="45"/>
-      <c r="GI3" s="45"/>
-      <c r="GJ3" s="36" t="s">
+      <c r="GB3" s="46"/>
+      <c r="GC3" s="46"/>
+      <c r="GD3" s="46"/>
+      <c r="GE3" s="46"/>
+      <c r="GF3" s="46"/>
+      <c r="GG3" s="46"/>
+      <c r="GH3" s="46"/>
+      <c r="GI3" s="46"/>
+      <c r="GJ3" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="GK3" s="36" t="s">
+      <c r="GK3" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="GL3" s="37"/>
-      <c r="GM3" s="37"/>
-      <c r="GN3" s="37"/>
-      <c r="GO3" s="37"/>
-      <c r="GP3" s="37"/>
-      <c r="GQ3" s="37"/>
-      <c r="GR3" s="37"/>
-      <c r="GS3" s="37"/>
+      <c r="GL3" s="38"/>
+      <c r="GM3" s="38"/>
+      <c r="GN3" s="38"/>
+      <c r="GO3" s="38"/>
+      <c r="GP3" s="38"/>
+      <c r="GQ3" s="38"/>
+      <c r="GR3" s="38"/>
+      <c r="GS3" s="38"/>
       <c r="GT3" s="33"/>
-      <c r="GU3" s="36" t="s">
+      <c r="GU3" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="GV3" s="36" t="s">
+      <c r="GV3" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="GW3" s="36" t="s">
+      <c r="GW3" s="37" t="s">
         <v>118</v>
       </c>
       <c r="GX3" s="8"/>
       <c r="GY3" s="9"/>
     </row>
     <row r="4" spans="1:207" ht="84.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="52"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
       <c r="D4" s="32" t="s">
         <v>119</v>
       </c>
@@ -3311,24 +3864,24 @@
       <c r="F4" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37"/>
-      <c r="W4" s="37"/>
-      <c r="X4" s="37"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="38"/>
+      <c r="W4" s="38"/>
+      <c r="X4" s="38"/>
       <c r="Y4" s="32" t="s">
         <v>119</v>
       </c>
@@ -3344,18 +3897,18 @@
       <c r="AC4" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="AD4" s="37"/>
-      <c r="AE4" s="37"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
       <c r="AF4" s="32" t="s">
         <v>40</v>
       </c>
       <c r="AG4" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="AH4" s="37"/>
-      <c r="AI4" s="37"/>
-      <c r="AJ4" s="37"/>
-      <c r="AK4" s="37"/>
+      <c r="AH4" s="38"/>
+      <c r="AI4" s="38"/>
+      <c r="AJ4" s="38"/>
+      <c r="AK4" s="38"/>
       <c r="AL4" s="32" t="s">
         <v>125</v>
       </c>
@@ -3380,9 +3933,9 @@
       <c r="AS4" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="AT4" s="37"/>
-      <c r="AU4" s="37"/>
-      <c r="AV4" s="37"/>
+      <c r="AT4" s="38"/>
+      <c r="AU4" s="38"/>
+      <c r="AV4" s="38"/>
       <c r="AW4" s="7" t="s">
         <v>127</v>
       </c>
@@ -3401,11 +3954,11 @@
       <c r="BB4" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="BC4" s="37"/>
-      <c r="BD4" s="37"/>
-      <c r="BE4" s="37"/>
-      <c r="BF4" s="37"/>
-      <c r="BG4" s="37"/>
+      <c r="BC4" s="38"/>
+      <c r="BD4" s="38"/>
+      <c r="BE4" s="38"/>
+      <c r="BF4" s="38"/>
+      <c r="BG4" s="38"/>
       <c r="BH4" s="7" t="s">
         <v>133</v>
       </c>
@@ -3415,7 +3968,7 @@
       <c r="BJ4" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="BK4" s="37"/>
+      <c r="BK4" s="38"/>
       <c r="BL4" s="32" t="s">
         <v>136</v>
       </c>
@@ -3455,7 +4008,7 @@
       <c r="BX4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="BY4" s="37"/>
+      <c r="BY4" s="38"/>
       <c r="BZ4" s="32" t="s">
         <v>147</v>
       </c>
@@ -3481,13 +4034,13 @@
       <c r="CH4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="CI4" s="37"/>
-      <c r="CJ4" s="37"/>
-      <c r="CK4" s="37"/>
-      <c r="CL4" s="37"/>
-      <c r="CM4" s="37"/>
-      <c r="CN4" s="37"/>
-      <c r="CO4" s="37"/>
+      <c r="CI4" s="38"/>
+      <c r="CJ4" s="38"/>
+      <c r="CK4" s="38"/>
+      <c r="CL4" s="38"/>
+      <c r="CM4" s="38"/>
+      <c r="CN4" s="38"/>
+      <c r="CO4" s="38"/>
       <c r="CP4" s="32" t="s">
         <v>151</v>
       </c>
@@ -3518,11 +4071,11 @@
       <c r="CY4" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="CZ4" s="37"/>
-      <c r="DA4" s="37"/>
-      <c r="DB4" s="37"/>
-      <c r="DC4" s="37"/>
-      <c r="DD4" s="37"/>
+      <c r="CZ4" s="38"/>
+      <c r="DA4" s="38"/>
+      <c r="DB4" s="38"/>
+      <c r="DC4" s="38"/>
+      <c r="DD4" s="38"/>
       <c r="DE4" s="32" t="s">
         <v>160</v>
       </c>
@@ -3559,13 +4112,13 @@
       <c r="DP4" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="DQ4" s="37"/>
-      <c r="DR4" s="37"/>
-      <c r="DS4" s="37"/>
-      <c r="DT4" s="37"/>
-      <c r="DU4" s="37"/>
-      <c r="DV4" s="37"/>
-      <c r="DW4" s="37"/>
+      <c r="DQ4" s="38"/>
+      <c r="DR4" s="38"/>
+      <c r="DS4" s="38"/>
+      <c r="DT4" s="38"/>
+      <c r="DU4" s="38"/>
+      <c r="DV4" s="38"/>
+      <c r="DW4" s="38"/>
       <c r="DX4" s="32" t="s">
         <v>163</v>
       </c>
@@ -3587,7 +4140,7 @@
       <c r="ED4" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="EE4" s="37"/>
+      <c r="EE4" s="38"/>
       <c r="EF4" s="32" t="s">
         <v>169</v>
       </c>
@@ -3648,7 +4201,7 @@
       <c r="EY4" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="EZ4" s="37"/>
+      <c r="EZ4" s="38"/>
       <c r="FA4" s="32" t="s">
         <v>172</v>
       </c>
@@ -3682,7 +4235,7 @@
       <c r="FK4" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="FL4" s="37"/>
+      <c r="FL4" s="38"/>
       <c r="FM4" s="32" t="s">
         <v>172</v>
       </c>
@@ -3716,9 +4269,9 @@
       <c r="FW4" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="FX4" s="37"/>
-      <c r="FY4" s="37"/>
-      <c r="FZ4" s="37"/>
+      <c r="FX4" s="38"/>
+      <c r="FY4" s="38"/>
+      <c r="FZ4" s="38"/>
       <c r="GA4" s="7" t="s">
         <v>182</v>
       </c>
@@ -3746,7 +4299,7 @@
       <c r="GI4" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="GJ4" s="37"/>
+      <c r="GJ4" s="38"/>
       <c r="GK4" s="7" t="s">
         <v>191</v>
       </c>
@@ -3775,9 +4328,9 @@
         <v>139</v>
       </c>
       <c r="GT4" s="33"/>
-      <c r="GU4" s="37"/>
-      <c r="GV4" s="37"/>
-      <c r="GW4" s="37"/>
+      <c r="GU4" s="38"/>
+      <c r="GV4" s="38"/>
+      <c r="GW4" s="38"/>
       <c r="GX4" s="12" t="s">
         <v>199</v>
       </c>
@@ -3827,8 +4380,8 @@
       <c r="AO5" s="15"/>
       <c r="AP5" s="15"/>
       <c r="AQ5" s="15"/>
-      <c r="AR5" s="49"/>
-      <c r="AS5" s="50"/>
+      <c r="AR5" s="50"/>
+      <c r="AS5" s="51"/>
       <c r="AT5" s="15"/>
       <c r="AU5" s="15"/>
       <c r="AV5" s="15"/>
@@ -3847,36 +4400,36 @@
       <c r="BI5" s="15"/>
       <c r="BJ5" s="15"/>
       <c r="BK5" s="15"/>
-      <c r="BL5" s="49"/>
-      <c r="BM5" s="50"/>
-      <c r="BN5" s="49"/>
-      <c r="BO5" s="61"/>
-      <c r="BP5" s="50"/>
+      <c r="BL5" s="50"/>
+      <c r="BM5" s="51"/>
+      <c r="BN5" s="50"/>
+      <c r="BO5" s="62"/>
+      <c r="BP5" s="51"/>
       <c r="BQ5" s="16"/>
       <c r="BR5" s="16"/>
       <c r="BS5" s="16"/>
       <c r="BT5" s="16"/>
       <c r="BU5" s="16"/>
       <c r="BV5" s="16"/>
-      <c r="BW5" s="49"/>
-      <c r="BX5" s="50"/>
+      <c r="BW5" s="50"/>
+      <c r="BX5" s="51"/>
       <c r="BY5" s="15"/>
-      <c r="BZ5" s="49"/>
-      <c r="CA5" s="50"/>
-      <c r="CB5" s="49"/>
-      <c r="CC5" s="50"/>
-      <c r="CD5" s="49"/>
-      <c r="CE5" s="50"/>
+      <c r="BZ5" s="50"/>
+      <c r="CA5" s="51"/>
+      <c r="CB5" s="50"/>
+      <c r="CC5" s="51"/>
+      <c r="CD5" s="50"/>
+      <c r="CE5" s="51"/>
       <c r="CF5" s="15"/>
-      <c r="CG5" s="49"/>
-      <c r="CH5" s="50"/>
+      <c r="CG5" s="50"/>
+      <c r="CH5" s="51"/>
       <c r="CI5" s="15"/>
       <c r="CJ5" s="15"/>
       <c r="CK5" s="15"/>
       <c r="CL5" s="15"/>
       <c r="CM5" s="15"/>
-      <c r="CN5" s="49"/>
-      <c r="CO5" s="50"/>
+      <c r="CN5" s="50"/>
+      <c r="CO5" s="51"/>
       <c r="CP5" s="16"/>
       <c r="CQ5" s="16"/>
       <c r="CR5" s="16"/>
@@ -3919,26 +4472,26 @@
       <c r="EC5" s="21"/>
       <c r="ED5" s="21"/>
       <c r="EE5" s="20"/>
-      <c r="EF5" s="59"/>
-      <c r="EG5" s="60"/>
-      <c r="EH5" s="59"/>
-      <c r="EI5" s="60"/>
-      <c r="EJ5" s="49"/>
-      <c r="EK5" s="50"/>
-      <c r="EL5" s="49"/>
-      <c r="EM5" s="50"/>
-      <c r="EN5" s="49"/>
-      <c r="EO5" s="50"/>
-      <c r="EP5" s="49"/>
-      <c r="EQ5" s="50"/>
-      <c r="ER5" s="49"/>
-      <c r="ES5" s="50"/>
-      <c r="ET5" s="49"/>
-      <c r="EU5" s="50"/>
-      <c r="EV5" s="49"/>
-      <c r="EW5" s="50"/>
-      <c r="EX5" s="49"/>
-      <c r="EY5" s="50"/>
+      <c r="EF5" s="60"/>
+      <c r="EG5" s="61"/>
+      <c r="EH5" s="60"/>
+      <c r="EI5" s="61"/>
+      <c r="EJ5" s="50"/>
+      <c r="EK5" s="51"/>
+      <c r="EL5" s="50"/>
+      <c r="EM5" s="51"/>
+      <c r="EN5" s="50"/>
+      <c r="EO5" s="51"/>
+      <c r="EP5" s="50"/>
+      <c r="EQ5" s="51"/>
+      <c r="ER5" s="50"/>
+      <c r="ES5" s="51"/>
+      <c r="ET5" s="50"/>
+      <c r="EU5" s="51"/>
+      <c r="EV5" s="50"/>
+      <c r="EW5" s="51"/>
+      <c r="EX5" s="50"/>
+      <c r="EY5" s="51"/>
       <c r="EZ5" s="15"/>
       <c r="FA5" s="16"/>
       <c r="FB5" s="16"/>
@@ -3963,8 +4516,8 @@
       <c r="FU5" s="16"/>
       <c r="FV5" s="16"/>
       <c r="FW5" s="16"/>
-      <c r="FX5" s="49"/>
-      <c r="FY5" s="50"/>
+      <c r="FX5" s="50"/>
+      <c r="FY5" s="51"/>
       <c r="FZ5" s="15"/>
       <c r="GA5" s="16"/>
       <c r="GB5" s="16"/>
@@ -3985,12 +4538,12 @@
       <c r="GQ5" s="16"/>
       <c r="GR5" s="16"/>
       <c r="GS5" s="16"/>
-      <c r="GT5" s="49"/>
-      <c r="GU5" s="61"/>
-      <c r="GV5" s="61"/>
-      <c r="GW5" s="61"/>
-      <c r="GX5" s="61"/>
-      <c r="GY5" s="50"/>
+      <c r="GT5" s="50"/>
+      <c r="GU5" s="62"/>
+      <c r="GV5" s="62"/>
+      <c r="GW5" s="62"/>
+      <c r="GX5" s="62"/>
+      <c r="GY5" s="51"/>
     </row>
     <row r="6" spans="1:207" ht="21.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22"/>
@@ -7803,6 +8356,7 @@
     <mergeCell ref="ET5:EU5"/>
     <mergeCell ref="DE3:DG3"/>
     <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="ER5:ES5"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="ET3:EU3"/>
     <mergeCell ref="AF2:BJ2"/>
@@ -7851,9 +8405,6 @@
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="DW3:DW4"/>
     <mergeCell ref="BZ5:CA5"/>
-    <mergeCell ref="ER5:ES5"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="DR3:DR4"/>
     <mergeCell ref="BF3:BF4"/>
     <mergeCell ref="AI3:AI4"/>
     <mergeCell ref="EP3:EQ3"/>
@@ -7892,6 +8443,8 @@
     <mergeCell ref="AF3:AG3"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="DU3:DU4"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="DR3:DR4"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup orientation="portrait"/>
@@ -7902,6 +8455,828 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:GU1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="17" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="18" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="14" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="18" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="18" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="11" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="28" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="16" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="34" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="28" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="9" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="29" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="23" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="34" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="47" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="52" bestFit="1" customWidth="1"/>
+    <col min="120" max="122" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="45.5" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="8" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="135" max="136" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="22" bestFit="1" customWidth="1"/>
+    <col min="145" max="145" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="24" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="31" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="155" max="155" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="156" max="156" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="157" max="157" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="159" max="159" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="160" max="160" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="161" max="161" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="29" bestFit="1" customWidth="1"/>
+    <col min="163" max="163" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="164" max="164" width="31" bestFit="1" customWidth="1"/>
+    <col min="165" max="165" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="30" bestFit="1" customWidth="1"/>
+    <col min="168" max="168" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="169" max="169" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="170" max="170" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="171" max="171" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="172" max="172" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="173" max="173" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="174" max="174" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="175" max="175" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="176" max="176" width="25" bestFit="1" customWidth="1"/>
+    <col min="177" max="177" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="178" max="178" width="21" bestFit="1" customWidth="1"/>
+    <col min="179" max="179" width="32.33203125" customWidth="1"/>
+    <col min="180" max="180" width="24" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="18.1640625" customWidth="1"/>
+    <col min="184" max="184" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="185" max="185" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="187" max="187" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="189" max="189" width="25" bestFit="1" customWidth="1"/>
+    <col min="190" max="190" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="191" max="191" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="192" max="192" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="24.5" customWidth="1"/>
+    <col min="194" max="194" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="195" max="195" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="196" max="196" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="197" max="197" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="198" max="198" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="199" max="199" width="12" bestFit="1" customWidth="1"/>
+    <col min="200" max="200" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="202" max="202" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:203" s="36" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="36" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>207</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>208</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>209</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="L1" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="M1" s="36" t="s">
+        <v>212</v>
+      </c>
+      <c r="N1" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="P1" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q1" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="R1" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="36" t="s">
+        <v>216</v>
+      </c>
+      <c r="V1" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="W1" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="Y1" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="Z1" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA1" s="36" t="s">
+        <v>221</v>
+      </c>
+      <c r="AB1" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="AC1" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD1" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="AE1" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="AF1" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="AG1" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="AH1" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="AI1" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="AJ1" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="AK1" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="AL1" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="AM1" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="AN1" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="AO1" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="AP1" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="AQ1" s="36" t="s">
+        <v>237</v>
+      </c>
+      <c r="AR1" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="AS1" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="AT1" s="36" t="s">
+        <v>240</v>
+      </c>
+      <c r="AU1" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="AV1" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="AW1" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="AX1" s="36" t="s">
+        <v>244</v>
+      </c>
+      <c r="AY1" s="36" t="s">
+        <v>245</v>
+      </c>
+      <c r="AZ1" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="BA1" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="BB1" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="BC1" s="36" t="s">
+        <v>249</v>
+      </c>
+      <c r="BD1" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="BE1" s="36" t="s">
+        <v>251</v>
+      </c>
+      <c r="BF1" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="BG1" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="BH1" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI1" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="BJ1" s="36" t="s">
+        <v>252</v>
+      </c>
+      <c r="BK1" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="BL1" s="36" t="s">
+        <v>254</v>
+      </c>
+      <c r="BM1" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="BN1" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="BO1" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="BP1" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="BQ1" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="BR1" s="36" t="s">
+        <v>259</v>
+      </c>
+      <c r="BS1" s="36" t="s">
+        <v>260</v>
+      </c>
+      <c r="BT1" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="BU1" s="36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BV1" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="BW1" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="BX1" s="36" t="s">
+        <v>208</v>
+      </c>
+      <c r="BY1" s="36" t="s">
+        <v>262</v>
+      </c>
+      <c r="BZ1" s="36" t="s">
+        <v>263</v>
+      </c>
+      <c r="CA1" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="CB1" s="36" t="s">
+        <v>265</v>
+      </c>
+      <c r="CC1" s="36" t="s">
+        <v>266</v>
+      </c>
+      <c r="CD1" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="CE1" s="36" t="s">
+        <v>268</v>
+      </c>
+      <c r="CF1" s="36" t="s">
+        <v>269</v>
+      </c>
+      <c r="CG1" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="CH1" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="CI1" s="36" t="s">
+        <v>272</v>
+      </c>
+      <c r="CJ1" s="36" t="s">
+        <v>273</v>
+      </c>
+      <c r="CK1" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="CL1" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="CM1" s="36" t="s">
+        <v>276</v>
+      </c>
+      <c r="CN1" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="CO1" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="CP1" s="36" t="s">
+        <v>279</v>
+      </c>
+      <c r="CQ1" s="36" t="s">
+        <v>208</v>
+      </c>
+      <c r="CR1" s="36" t="s">
+        <v>280</v>
+      </c>
+      <c r="CS1" s="36" t="s">
+        <v>281</v>
+      </c>
+      <c r="CT1" s="36" t="s">
+        <v>282</v>
+      </c>
+      <c r="CU1" s="36" t="s">
+        <v>283</v>
+      </c>
+      <c r="CV1" s="36" t="s">
+        <v>284</v>
+      </c>
+      <c r="CW1" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="CX1" s="36" t="s">
+        <v>286</v>
+      </c>
+      <c r="CY1" s="36" t="s">
+        <v>287</v>
+      </c>
+      <c r="CZ1" s="36" t="s">
+        <v>288</v>
+      </c>
+      <c r="DA1" s="36" t="s">
+        <v>208</v>
+      </c>
+      <c r="DB1" s="36" t="s">
+        <v>289</v>
+      </c>
+      <c r="DC1" s="36" t="s">
+        <v>290</v>
+      </c>
+      <c r="DD1" s="36" t="s">
+        <v>291</v>
+      </c>
+      <c r="DE1" s="36" t="s">
+        <v>292</v>
+      </c>
+      <c r="DF1" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="DG1" s="36" t="s">
+        <v>294</v>
+      </c>
+      <c r="DH1" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="DI1" s="36" t="s">
+        <v>296</v>
+      </c>
+      <c r="DJ1" s="36" t="s">
+        <v>297</v>
+      </c>
+      <c r="DK1" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="DL1" s="36" t="s">
+        <v>299</v>
+      </c>
+      <c r="DM1" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="DN1" s="36" t="s">
+        <v>301</v>
+      </c>
+      <c r="DO1" s="36" t="s">
+        <v>302</v>
+      </c>
+      <c r="DP1" s="36" t="s">
+        <v>303</v>
+      </c>
+      <c r="DQ1" s="36" t="s">
+        <v>381</v>
+      </c>
+      <c r="DR1" s="36" t="s">
+        <v>382</v>
+      </c>
+      <c r="DS1" s="36" t="s">
+        <v>304</v>
+      </c>
+      <c r="DT1" s="36" t="s">
+        <v>305</v>
+      </c>
+      <c r="DU1" s="36" t="s">
+        <v>306</v>
+      </c>
+      <c r="DV1" s="36" t="s">
+        <v>307</v>
+      </c>
+      <c r="DW1" s="36" t="s">
+        <v>308</v>
+      </c>
+      <c r="DX1" s="36" t="s">
+        <v>309</v>
+      </c>
+      <c r="DY1" s="36" t="s">
+        <v>310</v>
+      </c>
+      <c r="DZ1" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="EA1" s="36" t="s">
+        <v>311</v>
+      </c>
+      <c r="EB1" s="36" t="s">
+        <v>165</v>
+      </c>
+      <c r="EC1" s="36" t="s">
+        <v>312</v>
+      </c>
+      <c r="ED1" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="EE1" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="EF1" s="36" t="s">
+        <v>313</v>
+      </c>
+      <c r="EG1" s="36" t="s">
+        <v>314</v>
+      </c>
+      <c r="EH1" s="36" t="s">
+        <v>315</v>
+      </c>
+      <c r="EI1" s="36" t="s">
+        <v>316</v>
+      </c>
+      <c r="EJ1" s="36" t="s">
+        <v>317</v>
+      </c>
+      <c r="EK1" s="36" t="s">
+        <v>318</v>
+      </c>
+      <c r="EL1" s="36" t="s">
+        <v>319</v>
+      </c>
+      <c r="EM1" s="36" t="s">
+        <v>320</v>
+      </c>
+      <c r="EN1" s="36" t="s">
+        <v>321</v>
+      </c>
+      <c r="EO1" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="EP1" s="36" t="s">
+        <v>323</v>
+      </c>
+      <c r="EQ1" s="36" t="s">
+        <v>324</v>
+      </c>
+      <c r="ER1" s="36" t="s">
+        <v>325</v>
+      </c>
+      <c r="ES1" s="36" t="s">
+        <v>326</v>
+      </c>
+      <c r="ET1" s="36" t="s">
+        <v>327</v>
+      </c>
+      <c r="EU1" s="36" t="s">
+        <v>328</v>
+      </c>
+      <c r="EV1" s="36" t="s">
+        <v>329</v>
+      </c>
+      <c r="EW1" s="36" t="s">
+        <v>330</v>
+      </c>
+      <c r="EX1" s="36" t="s">
+        <v>331</v>
+      </c>
+      <c r="EY1" s="36" t="s">
+        <v>332</v>
+      </c>
+      <c r="EZ1" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="FA1" s="36" t="s">
+        <v>334</v>
+      </c>
+      <c r="FB1" s="36" t="s">
+        <v>335</v>
+      </c>
+      <c r="FC1" s="36" t="s">
+        <v>336</v>
+      </c>
+      <c r="FD1" s="36" t="s">
+        <v>337</v>
+      </c>
+      <c r="FE1" s="36" t="s">
+        <v>338</v>
+      </c>
+      <c r="FF1" s="36" t="s">
+        <v>339</v>
+      </c>
+      <c r="FG1" s="36" t="s">
+        <v>340</v>
+      </c>
+      <c r="FH1" s="36" t="s">
+        <v>341</v>
+      </c>
+      <c r="FI1" s="36" t="s">
+        <v>342</v>
+      </c>
+      <c r="FJ1" s="36" t="s">
+        <v>343</v>
+      </c>
+      <c r="FK1" s="36" t="s">
+        <v>344</v>
+      </c>
+      <c r="FL1" s="36" t="s">
+        <v>345</v>
+      </c>
+      <c r="FM1" s="36" t="s">
+        <v>346</v>
+      </c>
+      <c r="FN1" s="36" t="s">
+        <v>347</v>
+      </c>
+      <c r="FO1" s="36" t="s">
+        <v>348</v>
+      </c>
+      <c r="FP1" s="36" t="s">
+        <v>349</v>
+      </c>
+      <c r="FQ1" s="36" t="s">
+        <v>350</v>
+      </c>
+      <c r="FR1" s="36" t="s">
+        <v>351</v>
+      </c>
+      <c r="FS1" s="36" t="s">
+        <v>352</v>
+      </c>
+      <c r="FT1" s="36" t="s">
+        <v>353</v>
+      </c>
+      <c r="FU1" s="36" t="s">
+        <v>354</v>
+      </c>
+      <c r="FV1" s="36" t="s">
+        <v>355</v>
+      </c>
+      <c r="FW1" s="36" t="s">
+        <v>356</v>
+      </c>
+      <c r="FX1" s="36" t="s">
+        <v>357</v>
+      </c>
+      <c r="FY1" s="36" t="s">
+        <v>358</v>
+      </c>
+      <c r="FZ1" s="36" t="s">
+        <v>359</v>
+      </c>
+      <c r="GA1" s="36" t="s">
+        <v>379</v>
+      </c>
+      <c r="GB1" s="36" t="s">
+        <v>360</v>
+      </c>
+      <c r="GC1" s="36" t="s">
+        <v>361</v>
+      </c>
+      <c r="GD1" s="36" t="s">
+        <v>362</v>
+      </c>
+      <c r="GE1" s="36" t="s">
+        <v>363</v>
+      </c>
+      <c r="GF1" s="36" t="s">
+        <v>364</v>
+      </c>
+      <c r="GG1" s="36" t="s">
+        <v>365</v>
+      </c>
+      <c r="GH1" s="36" t="s">
+        <v>366</v>
+      </c>
+      <c r="GI1" s="36" t="s">
+        <v>367</v>
+      </c>
+      <c r="GJ1" s="36" t="s">
+        <v>368</v>
+      </c>
+      <c r="GK1" s="36" t="s">
+        <v>380</v>
+      </c>
+      <c r="GL1" s="36" t="s">
+        <v>369</v>
+      </c>
+      <c r="GM1" s="36" t="s">
+        <v>370</v>
+      </c>
+      <c r="GN1" s="36" t="s">
+        <v>371</v>
+      </c>
+      <c r="GO1" s="36" t="s">
+        <v>372</v>
+      </c>
+      <c r="GP1" s="36" t="s">
+        <v>373</v>
+      </c>
+      <c r="GQ1" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="GR1" s="36" t="s">
+        <v>375</v>
+      </c>
+      <c r="GS1" s="36" t="s">
+        <v>376</v>
+      </c>
+      <c r="GT1" s="36" t="s">
+        <v>377</v>
+      </c>
+      <c r="GU1" s="36" t="s">
+        <v>378</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G132"/>
   <sheetViews>
@@ -7924,95 +9299,95 @@
       <c r="D1" s="28"/>
     </row>
     <row r="2" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="D2" s="68"/>
-      <c r="E2" s="66"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="D3" s="68"/>
-      <c r="E3" s="66"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="67"/>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="D4" s="68"/>
-      <c r="E4" s="66"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="67"/>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="D5" s="68"/>
-      <c r="E5" s="66"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="67"/>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="D6" s="68"/>
-      <c r="E6" s="66"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="67"/>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="D7" s="68"/>
-      <c r="E7" s="66"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="67"/>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="D8" s="68"/>
-      <c r="E8" s="66"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="67"/>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="D9" s="68"/>
+      <c r="D9" s="69"/>
     </row>
     <row r="10" spans="3:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="67"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="68"/>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="67"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="68"/>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="67"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="68"/>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="67"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="68"/>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="67"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="68"/>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="67"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="68"/>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="67"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="68"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="67"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="68"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="67"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="68"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="67"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="68"/>
     </row>
     <row r="21" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="29"/>
@@ -8021,83 +9396,83 @@
       <c r="D21" s="29"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="E22" s="65"/>
+      <c r="E22" s="66"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D23" s="68"/>
-      <c r="E23" s="65"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="66"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D24" s="68"/>
-      <c r="E24" s="65"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="66"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D25" s="68"/>
-      <c r="E25" s="65"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="66"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C26" s="65"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="65"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="66"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C27" s="65"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="65"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="66"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C28" s="65"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="65"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="66"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C29" s="65"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="65"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="66"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C30" s="65"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="65"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="66"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C31" s="65"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="65"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="66"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C32" s="65"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="65"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="66"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C33" s="65"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="65"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="66"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C34" s="65"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="65"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="66"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C35" s="65"/>
-      <c r="D35" s="68"/>
-      <c r="E35" s="65"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="66"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C36" s="65"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="65"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="66"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C37" s="65"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="65"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="66"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D38" s="68"/>
-      <c r="E38" s="65"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="66"/>
     </row>
     <row r="39" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="29"/>
@@ -8107,92 +9482,92 @@
       <c r="E39" s="34"/>
     </row>
     <row r="40" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D40" s="68"/>
-      <c r="E40" s="67"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="68"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D41" s="68"/>
-      <c r="E41" s="67"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="68"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D42" s="68"/>
-      <c r="E42" s="67"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="68"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D43" s="68"/>
-      <c r="E43" s="67"/>
+      <c r="D43" s="69"/>
+      <c r="E43" s="68"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D44" s="68"/>
-      <c r="E44" s="67"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="68"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D45" s="68"/>
-      <c r="E45" s="67"/>
+      <c r="D45" s="69"/>
+      <c r="E45" s="68"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C46" s="69"/>
-      <c r="D46" s="68"/>
-      <c r="E46" s="68"/>
-      <c r="F46" s="65"/>
+      <c r="C46" s="70"/>
+      <c r="D46" s="69"/>
+      <c r="E46" s="69"/>
+      <c r="F46" s="66"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C47" s="69"/>
-      <c r="D47" s="68"/>
-      <c r="E47" s="68"/>
-      <c r="F47" s="65"/>
+      <c r="C47" s="70"/>
+      <c r="D47" s="69"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="66"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C48" s="69"/>
-      <c r="D48" s="68"/>
-      <c r="E48" s="68"/>
-      <c r="F48" s="65"/>
+      <c r="C48" s="70"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="69"/>
+      <c r="F48" s="66"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C49" s="69"/>
-      <c r="D49" s="68"/>
-      <c r="E49" s="68"/>
-      <c r="F49" s="65"/>
+      <c r="C49" s="70"/>
+      <c r="D49" s="69"/>
+      <c r="E49" s="69"/>
+      <c r="F49" s="66"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C50" s="69"/>
-      <c r="D50" s="68"/>
-      <c r="E50" s="68"/>
-      <c r="F50" s="65"/>
+      <c r="C50" s="70"/>
+      <c r="D50" s="69"/>
+      <c r="E50" s="69"/>
+      <c r="F50" s="66"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C51" s="69"/>
-      <c r="D51" s="68"/>
-      <c r="E51" s="68"/>
-      <c r="F51" s="65"/>
+      <c r="C51" s="70"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="66"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C52" s="69"/>
-      <c r="D52" s="68"/>
+      <c r="C52" s="70"/>
+      <c r="D52" s="69"/>
       <c r="E52" s="34"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D53" s="68"/>
+      <c r="D53" s="69"/>
       <c r="E53" s="34"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C54" s="67"/>
-      <c r="D54" s="68"/>
+      <c r="C54" s="68"/>
+      <c r="D54" s="69"/>
       <c r="E54" s="34"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C55" s="67"/>
-      <c r="D55" s="68"/>
+      <c r="C55" s="68"/>
+      <c r="D55" s="69"/>
       <c r="E55" s="34"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C56" s="67"/>
-      <c r="D56" s="68"/>
+      <c r="C56" s="68"/>
+      <c r="D56" s="69"/>
       <c r="E56" s="34"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C57" s="67"/>
-      <c r="D57" s="68"/>
+      <c r="C57" s="68"/>
+      <c r="D57" s="69"/>
       <c r="E57" s="34"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
@@ -8202,223 +9577,223 @@
       <c r="D58" s="30"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C59" s="65"/>
-      <c r="D59" s="68"/>
-      <c r="E59" s="65"/>
+      <c r="C59" s="66"/>
+      <c r="D59" s="69"/>
+      <c r="E59" s="66"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C60" s="65"/>
-      <c r="D60" s="68"/>
-      <c r="E60" s="65"/>
+      <c r="C60" s="66"/>
+      <c r="D60" s="69"/>
+      <c r="E60" s="66"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C61" s="65"/>
-      <c r="D61" s="68"/>
-      <c r="E61" s="65"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="69"/>
+      <c r="E61" s="66"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C62" s="65"/>
-      <c r="D62" s="68"/>
-      <c r="E62" s="65"/>
+      <c r="C62" s="66"/>
+      <c r="D62" s="69"/>
+      <c r="E62" s="66"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C63" s="65"/>
-      <c r="D63" s="68"/>
-      <c r="E63" s="65"/>
+      <c r="C63" s="66"/>
+      <c r="D63" s="69"/>
+      <c r="E63" s="66"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C64" s="65"/>
-      <c r="D64" s="68"/>
-      <c r="E64" s="65"/>
+      <c r="C64" s="66"/>
+      <c r="D64" s="69"/>
+      <c r="E64" s="66"/>
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C65" s="65"/>
-      <c r="D65" s="68"/>
-      <c r="E65" s="65"/>
+      <c r="C65" s="66"/>
+      <c r="D65" s="69"/>
+      <c r="E65" s="66"/>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C66" s="65"/>
-      <c r="D66" s="68"/>
-      <c r="E66" s="65"/>
+      <c r="C66" s="66"/>
+      <c r="D66" s="69"/>
+      <c r="E66" s="66"/>
     </row>
     <row r="67" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C67" s="65"/>
-      <c r="D67" s="68"/>
-      <c r="E67" s="65"/>
+      <c r="C67" s="66"/>
+      <c r="D67" s="69"/>
+      <c r="E67" s="66"/>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C68" s="65"/>
-      <c r="D68" s="68"/>
-      <c r="E68" s="65"/>
+      <c r="C68" s="66"/>
+      <c r="D68" s="69"/>
+      <c r="E68" s="66"/>
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C69" s="65"/>
-      <c r="D69" s="68"/>
-      <c r="E69" s="65"/>
+      <c r="C69" s="66"/>
+      <c r="D69" s="69"/>
+      <c r="E69" s="66"/>
     </row>
     <row r="70" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C70" s="65"/>
-      <c r="D70" s="68"/>
-      <c r="E70" s="65"/>
+      <c r="C70" s="66"/>
+      <c r="D70" s="69"/>
+      <c r="E70" s="66"/>
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C71" s="65"/>
-      <c r="D71" s="68"/>
-      <c r="E71" s="65"/>
+      <c r="C71" s="66"/>
+      <c r="D71" s="69"/>
+      <c r="E71" s="66"/>
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C72" s="65"/>
-      <c r="D72" s="68"/>
-      <c r="E72" s="65"/>
+      <c r="C72" s="66"/>
+      <c r="D72" s="69"/>
+      <c r="E72" s="66"/>
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C73" s="65"/>
-      <c r="D73" s="68"/>
-      <c r="E73" s="65"/>
+      <c r="C73" s="66"/>
+      <c r="D73" s="69"/>
+      <c r="E73" s="66"/>
     </row>
     <row r="74" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C74" s="65"/>
-      <c r="D74" s="68"/>
-      <c r="E74" s="65"/>
+      <c r="C74" s="66"/>
+      <c r="D74" s="69"/>
+      <c r="E74" s="66"/>
     </row>
     <row r="75" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="D75" s="68"/>
-      <c r="E75" s="65"/>
+      <c r="D75" s="69"/>
+      <c r="E75" s="66"/>
     </row>
     <row r="76" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C76" s="65"/>
-      <c r="D76" s="68"/>
-      <c r="E76" s="65"/>
-      <c r="F76" s="65"/>
+      <c r="C76" s="66"/>
+      <c r="D76" s="69"/>
+      <c r="E76" s="66"/>
+      <c r="F76" s="66"/>
     </row>
     <row r="77" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C77" s="65"/>
-      <c r="D77" s="68"/>
-      <c r="E77" s="65"/>
-      <c r="F77" s="65"/>
+      <c r="C77" s="66"/>
+      <c r="D77" s="69"/>
+      <c r="E77" s="66"/>
+      <c r="F77" s="66"/>
     </row>
     <row r="78" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C78" s="65"/>
-      <c r="D78" s="68"/>
-      <c r="E78" s="65"/>
-      <c r="F78" s="65"/>
+      <c r="C78" s="66"/>
+      <c r="D78" s="69"/>
+      <c r="E78" s="66"/>
+      <c r="F78" s="66"/>
     </row>
     <row r="79" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C79" s="65"/>
-      <c r="D79" s="68"/>
-      <c r="E79" s="65"/>
-      <c r="F79" s="65"/>
+      <c r="C79" s="66"/>
+      <c r="D79" s="69"/>
+      <c r="E79" s="66"/>
+      <c r="F79" s="66"/>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C80" s="65"/>
-      <c r="D80" s="68"/>
-      <c r="E80" s="65"/>
-      <c r="F80" s="65"/>
+      <c r="C80" s="66"/>
+      <c r="D80" s="69"/>
+      <c r="E80" s="66"/>
+      <c r="F80" s="66"/>
     </row>
     <row r="81" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C81" s="65"/>
-      <c r="D81" s="68"/>
-      <c r="E81" s="65"/>
-      <c r="F81" s="65"/>
+      <c r="C81" s="66"/>
+      <c r="D81" s="69"/>
+      <c r="E81" s="66"/>
+      <c r="F81" s="66"/>
     </row>
     <row r="82" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C82" s="65"/>
-      <c r="D82" s="68"/>
-      <c r="E82" s="65"/>
-      <c r="F82" s="65"/>
+      <c r="C82" s="66"/>
+      <c r="D82" s="69"/>
+      <c r="E82" s="66"/>
+      <c r="F82" s="66"/>
     </row>
     <row r="83" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C83" s="65"/>
-      <c r="D83" s="68"/>
-      <c r="E83" s="65"/>
-      <c r="F83" s="65"/>
+      <c r="C83" s="66"/>
+      <c r="D83" s="69"/>
+      <c r="E83" s="66"/>
+      <c r="F83" s="66"/>
     </row>
     <row r="84" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C84" s="65"/>
-      <c r="D84" s="68"/>
-      <c r="E84" s="65"/>
-      <c r="F84" s="65"/>
+      <c r="C84" s="66"/>
+      <c r="D84" s="69"/>
+      <c r="E84" s="66"/>
+      <c r="F84" s="66"/>
     </row>
     <row r="85" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C85" s="65"/>
-      <c r="D85" s="68"/>
-      <c r="E85" s="65"/>
-      <c r="F85" s="65"/>
+      <c r="C85" s="66"/>
+      <c r="D85" s="69"/>
+      <c r="E85" s="66"/>
+      <c r="F85" s="66"/>
     </row>
     <row r="86" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C86" s="65"/>
-      <c r="D86" s="68"/>
-      <c r="E86" s="65"/>
-      <c r="F86" s="65"/>
+      <c r="C86" s="66"/>
+      <c r="D86" s="69"/>
+      <c r="E86" s="66"/>
+      <c r="F86" s="66"/>
     </row>
     <row r="87" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="D87" s="68"/>
+      <c r="D87" s="69"/>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C88" s="65"/>
-      <c r="D88" s="68"/>
-      <c r="E88" s="65"/>
-      <c r="F88" s="65"/>
+      <c r="C88" s="66"/>
+      <c r="D88" s="69"/>
+      <c r="E88" s="66"/>
+      <c r="F88" s="66"/>
     </row>
     <row r="89" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C89" s="65"/>
-      <c r="D89" s="68"/>
-      <c r="E89" s="65"/>
-      <c r="F89" s="65"/>
+      <c r="C89" s="66"/>
+      <c r="D89" s="69"/>
+      <c r="E89" s="66"/>
+      <c r="F89" s="66"/>
     </row>
     <row r="90" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C90" s="65"/>
-      <c r="D90" s="68"/>
-      <c r="E90" s="65"/>
-      <c r="F90" s="65"/>
+      <c r="C90" s="66"/>
+      <c r="D90" s="69"/>
+      <c r="E90" s="66"/>
+      <c r="F90" s="66"/>
     </row>
     <row r="91" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C91" s="65"/>
-      <c r="D91" s="68"/>
-      <c r="E91" s="65"/>
-      <c r="F91" s="65"/>
+      <c r="C91" s="66"/>
+      <c r="D91" s="69"/>
+      <c r="E91" s="66"/>
+      <c r="F91" s="66"/>
     </row>
     <row r="92" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C92" s="65"/>
-      <c r="D92" s="68"/>
-      <c r="E92" s="65"/>
-      <c r="F92" s="65"/>
+      <c r="C92" s="66"/>
+      <c r="D92" s="69"/>
+      <c r="E92" s="66"/>
+      <c r="F92" s="66"/>
     </row>
     <row r="93" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C93" s="65"/>
-      <c r="D93" s="68"/>
-      <c r="E93" s="65"/>
-      <c r="F93" s="65"/>
+      <c r="C93" s="66"/>
+      <c r="D93" s="69"/>
+      <c r="E93" s="66"/>
+      <c r="F93" s="66"/>
     </row>
     <row r="94" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C94" s="65"/>
-      <c r="D94" s="68"/>
-      <c r="E94" s="65"/>
-      <c r="F94" s="65"/>
+      <c r="C94" s="66"/>
+      <c r="D94" s="69"/>
+      <c r="E94" s="66"/>
+      <c r="F94" s="66"/>
     </row>
     <row r="95" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C95" s="65"/>
-      <c r="D95" s="68"/>
-      <c r="E95" s="65"/>
-      <c r="F95" s="65"/>
+      <c r="C95" s="66"/>
+      <c r="D95" s="69"/>
+      <c r="E95" s="66"/>
+      <c r="F95" s="66"/>
     </row>
     <row r="96" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C96" s="65"/>
-      <c r="D96" s="68"/>
-      <c r="E96" s="65"/>
-      <c r="F96" s="65"/>
+      <c r="C96" s="66"/>
+      <c r="D96" s="69"/>
+      <c r="E96" s="66"/>
+      <c r="F96" s="66"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C97" s="65"/>
-      <c r="D97" s="68"/>
-      <c r="E97" s="65"/>
-      <c r="F97" s="65"/>
+      <c r="C97" s="66"/>
+      <c r="D97" s="69"/>
+      <c r="E97" s="66"/>
+      <c r="F97" s="66"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C98" s="65"/>
-      <c r="D98" s="68"/>
-      <c r="E98" s="65"/>
-      <c r="F98" s="65"/>
+      <c r="C98" s="66"/>
+      <c r="D98" s="69"/>
+      <c r="E98" s="66"/>
+      <c r="F98" s="66"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A99" s="30"/>
@@ -8427,68 +9802,68 @@
       <c r="D99" s="30"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D100" s="65"/>
+      <c r="D100" s="66"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D101" s="65"/>
+      <c r="D101" s="66"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D102" s="65"/>
+      <c r="D102" s="66"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C103" s="65"/>
-      <c r="D103" s="65"/>
-      <c r="E103" s="65"/>
-      <c r="F103" s="65"/>
+      <c r="C103" s="66"/>
+      <c r="D103" s="66"/>
+      <c r="E103" s="66"/>
+      <c r="F103" s="66"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C104" s="65"/>
-      <c r="D104" s="65"/>
-      <c r="E104" s="65"/>
-      <c r="F104" s="65"/>
+      <c r="C104" s="66"/>
+      <c r="D104" s="66"/>
+      <c r="E104" s="66"/>
+      <c r="F104" s="66"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C105" s="65"/>
-      <c r="D105" s="65"/>
-      <c r="E105" s="65"/>
-      <c r="F105" s="65"/>
+      <c r="C105" s="66"/>
+      <c r="D105" s="66"/>
+      <c r="E105" s="66"/>
+      <c r="F105" s="66"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C106" s="65"/>
-      <c r="D106" s="65"/>
-      <c r="E106" s="65"/>
-      <c r="F106" s="65"/>
+      <c r="C106" s="66"/>
+      <c r="D106" s="66"/>
+      <c r="E106" s="66"/>
+      <c r="F106" s="66"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C107" s="65"/>
-      <c r="D107" s="65"/>
-      <c r="E107" s="65"/>
-      <c r="F107" s="65"/>
+      <c r="C107" s="66"/>
+      <c r="D107" s="66"/>
+      <c r="E107" s="66"/>
+      <c r="F107" s="66"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C108" s="65"/>
-      <c r="D108" s="65"/>
-      <c r="E108" s="65"/>
-      <c r="F108" s="65"/>
+      <c r="C108" s="66"/>
+      <c r="D108" s="66"/>
+      <c r="E108" s="66"/>
+      <c r="F108" s="66"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C109" s="65"/>
-      <c r="D109" s="65"/>
-      <c r="E109" s="65"/>
-      <c r="F109" s="65"/>
+      <c r="C109" s="66"/>
+      <c r="D109" s="66"/>
+      <c r="E109" s="66"/>
+      <c r="F109" s="66"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C110" s="65"/>
-      <c r="D110" s="65"/>
-      <c r="E110" s="65"/>
-      <c r="F110" s="65"/>
+      <c r="C110" s="66"/>
+      <c r="D110" s="66"/>
+      <c r="E110" s="66"/>
+      <c r="F110" s="66"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C111" s="65"/>
-      <c r="D111" s="65"/>
+      <c r="C111" s="66"/>
+      <c r="D111" s="66"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D112" s="65"/>
+      <c r="D112" s="66"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A113" s="30"/>
@@ -8497,56 +9872,56 @@
       <c r="D113" s="30"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C114" s="68"/>
-      <c r="D114" s="65"/>
-      <c r="E114" s="65"/>
-      <c r="F114" s="65"/>
+      <c r="C114" s="69"/>
+      <c r="D114" s="66"/>
+      <c r="E114" s="66"/>
+      <c r="F114" s="66"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C115" s="68"/>
-      <c r="D115" s="65"/>
-      <c r="E115" s="65"/>
-      <c r="F115" s="65"/>
+      <c r="C115" s="69"/>
+      <c r="D115" s="66"/>
+      <c r="E115" s="66"/>
+      <c r="F115" s="66"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C116" s="68"/>
-      <c r="D116" s="65"/>
-      <c r="E116" s="65"/>
-      <c r="F116" s="65"/>
+      <c r="C116" s="69"/>
+      <c r="D116" s="66"/>
+      <c r="E116" s="66"/>
+      <c r="F116" s="66"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C117" s="68"/>
-      <c r="D117" s="65"/>
-      <c r="E117" s="65"/>
-      <c r="F117" s="65"/>
+      <c r="C117" s="69"/>
+      <c r="D117" s="66"/>
+      <c r="E117" s="66"/>
+      <c r="F117" s="66"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C118" s="68"/>
-      <c r="D118" s="65"/>
-      <c r="E118" s="65"/>
-      <c r="F118" s="65"/>
+      <c r="C118" s="69"/>
+      <c r="D118" s="66"/>
+      <c r="E118" s="66"/>
+      <c r="F118" s="66"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C119" s="68"/>
-      <c r="D119" s="65"/>
-      <c r="E119" s="65"/>
-      <c r="F119" s="65"/>
+      <c r="C119" s="69"/>
+      <c r="D119" s="66"/>
+      <c r="E119" s="66"/>
+      <c r="F119" s="66"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C120" s="68"/>
-      <c r="D120" s="65"/>
-      <c r="E120" s="65"/>
-      <c r="F120" s="65"/>
+      <c r="C120" s="69"/>
+      <c r="D120" s="66"/>
+      <c r="E120" s="66"/>
+      <c r="F120" s="66"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C121" s="68"/>
-      <c r="D121" s="65"/>
-      <c r="E121" s="65"/>
-      <c r="F121" s="65"/>
+      <c r="C121" s="69"/>
+      <c r="D121" s="66"/>
+      <c r="E121" s="66"/>
+      <c r="F121" s="66"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="C122" s="68"/>
-      <c r="D122" s="65"/>
+      <c r="C122" s="69"/>
+      <c r="D122" s="66"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A123" s="30"/>
@@ -8561,16 +9936,16 @@
       <c r="D126" s="30"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D127" s="65"/>
+      <c r="D127" s="66"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="D128" s="65"/>
+      <c r="D128" s="66"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="D129" s="65"/>
+      <c r="D129" s="66"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="D130" s="65"/>
+      <c r="D130" s="66"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A132" s="30"/>
@@ -8590,25 +9965,25 @@
     <mergeCell ref="C29:C31"/>
     <mergeCell ref="C26:C28"/>
     <mergeCell ref="D23:D38"/>
-    <mergeCell ref="C114:C122"/>
-    <mergeCell ref="D114:D122"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C73:C74"/>
     <mergeCell ref="C76:C86"/>
-    <mergeCell ref="E88:E98"/>
-    <mergeCell ref="F88:F98"/>
     <mergeCell ref="C88:C98"/>
     <mergeCell ref="D59:D98"/>
     <mergeCell ref="C103:C111"/>
     <mergeCell ref="D100:D112"/>
     <mergeCell ref="C59:C60"/>
     <mergeCell ref="C61:C62"/>
-    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="E88:E98"/>
     <mergeCell ref="F103:F110"/>
     <mergeCell ref="E103:E110"/>
+    <mergeCell ref="C114:C122"/>
+    <mergeCell ref="D114:D122"/>
+    <mergeCell ref="F88:F98"/>
+    <mergeCell ref="C63:C64"/>
     <mergeCell ref="D127:D130"/>
     <mergeCell ref="E2:E8"/>
     <mergeCell ref="E10:E19"/>

</xml_diff>

<commit_message>
adding exit columns, voiding in exports
</commit_message>
<xml_diff>
--- a/templates/excel_template/dreams_export.xlsx
+++ b/templates/excel_template/dreams_export.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="202">
   <si>
     <t>County</t>
   </si>
@@ -624,6 +624,15 @@
   </si>
   <si>
     <t>Use_of_condom_with_Partner_Third_Last_Sexual_partner</t>
+  </si>
+  <si>
+    <t>exit_status</t>
+  </si>
+  <si>
+    <t>exit_date</t>
+  </si>
+  <si>
+    <t>exit_reason</t>
   </si>
 </sst>
 </file>
@@ -1871,7 +1880,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GU1"/>
+  <dimension ref="A1:GX1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2075,10 +2084,10 @@
     <col min="200" max="200" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="201" max="201" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="202" max="202" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="10" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:203" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:206" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -2684,6 +2693,15 @@
       </c>
       <c r="GU1" s="1" t="s">
         <v>194</v>
+      </c>
+      <c r="GV1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="GW1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="GX1" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>